<commit_message>
faceDetector and ProfileDetector now work properly in OSGi, refactored code to common superclass
</commit_message>
<xml_diff>
--- a/doc/flo/Blocks.xlsx
+++ b/doc/flo/Blocks.xlsx
@@ -665,14 +665,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -977,10 +977,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E24" workbookViewId="0">
-      <pane xSplit="11325" ySplit="6240" topLeftCell="AT49" activePane="topRight"/>
-      <selection activeCell="E42" sqref="A42:XFD42"/>
-      <selection pane="topRight" activeCell="AT43" sqref="AT43"/>
+    <sheetView tabSelected="1" topLeftCell="W21" workbookViewId="0">
+      <pane xSplit="11325" ySplit="6240" topLeftCell="AS49" activePane="topRight"/>
+      <selection activeCell="Z3" sqref="Z3"/>
+      <selection pane="topRight" activeCell="AT25" sqref="AT25"/>
       <selection pane="bottomLeft" activeCell="O56" sqref="O56"/>
       <selection pane="bottomRight" activeCell="AH55" sqref="AH55"/>
     </sheetView>
@@ -1007,10 +1007,10 @@
     <col min="31" max="31" width="32.7109375" customWidth="1"/>
     <col min="34" max="34" width="36.140625" customWidth="1"/>
     <col min="35" max="37" width="9.85546875" customWidth="1"/>
-    <col min="38" max="38" width="9" style="12" customWidth="1"/>
+    <col min="38" max="38" width="9" style="11" customWidth="1"/>
     <col min="39" max="39" width="8.28515625" customWidth="1"/>
     <col min="40" max="40" width="8.5703125" customWidth="1"/>
-    <col min="41" max="41" width="9.42578125" style="12" customWidth="1"/>
+    <col min="41" max="41" width="9.42578125" style="11" customWidth="1"/>
     <col min="42" max="42" width="24" customWidth="1"/>
     <col min="45" max="45" width="23.7109375" customWidth="1"/>
     <col min="46" max="46" width="87.7109375" customWidth="1"/>
@@ -1020,28 +1020,28 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10" t="s">
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10" t="s">
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
       <c r="T1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1074,10 +1074,10 @@
         <v>Control</v>
       </c>
       <c r="I2" s="3"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1102,16 +1102,16 @@
         <v>9</v>
       </c>
       <c r="I3" s="3"/>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="M3" s="11"/>
+      <c r="M3" s="10"/>
       <c r="N3" s="4" t="s">
         <v>10</v>
       </c>
@@ -1184,7 +1184,7 @@
         <f t="shared" ref="AK3:AL3" si="2">IF(ISBLANK(L3), "", ", "&amp;L3)</f>
         <v>, object</v>
       </c>
-      <c r="AL3" s="12" t="str">
+      <c r="AL3" s="11" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -1196,7 +1196,7 @@
         <f>IF(ISBLANK(R3), "", ", "&amp;R3)</f>
         <v/>
       </c>
-      <c r="AO3" s="12" t="str">
+      <c r="AO3" s="11" t="str">
         <f>IF(ISBLANK(S3), "", ", "&amp;S3)</f>
         <v/>
       </c>
@@ -1234,16 +1234,16 @@
         <v>9</v>
       </c>
       <c r="I4" s="3"/>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="M4" s="11"/>
+      <c r="M4" s="10"/>
       <c r="N4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1317,7 +1317,7 @@
         <f t="shared" ref="AK4:AK53" si="17">IF(ISBLANK(L4), "", ", "&amp;L4)</f>
         <v>, object</v>
       </c>
-      <c r="AL4" s="12" t="str">
+      <c r="AL4" s="11" t="str">
         <f t="shared" ref="AL4:AL53" si="18">IF(ISBLANK(M4), "", ", "&amp;M4)</f>
         <v/>
       </c>
@@ -1329,7 +1329,7 @@
         <f t="shared" ref="AN4:AN53" si="20">IF(ISBLANK(R4), "", ", "&amp;R4)</f>
         <v/>
       </c>
-      <c r="AO4" s="12" t="str">
+      <c r="AO4" s="11" t="str">
         <f t="shared" ref="AO4:AO53" si="21">IF(ISBLANK(S4), "", ", "&amp;S4)</f>
         <v/>
       </c>
@@ -1364,14 +1364,14 @@
         <v>16</v>
       </c>
       <c r="I5" s="3"/>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
       <c r="N5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1445,7 +1445,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL5" s="12" t="str">
+      <c r="AL5" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -1457,7 +1457,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO5" s="12" t="str">
+      <c r="AO5" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -1486,10 +1486,10 @@
         <v>Editor Support</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
       <c r="N6" s="4"/>
       <c r="V6" s="9" t="str">
         <f t="shared" si="3"/>
@@ -1555,7 +1555,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL6" s="12" t="str">
+      <c r="AL6" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -1567,7 +1567,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO6" s="12" t="str">
+      <c r="AO6" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -1599,14 +1599,14 @@
         <v>20</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
       <c r="N7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1680,7 +1680,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL7" s="12" t="str">
+      <c r="AL7" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -1692,7 +1692,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO7" s="12" t="str">
+      <c r="AO7" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -1721,10 +1721,10 @@
         <v>22</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
       <c r="N8" s="4" t="s">
         <v>10</v>
       </c>
@@ -1801,7 +1801,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL8" s="12" t="str">
+      <c r="AL8" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -1813,7 +1813,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO8" s="12" t="str">
+      <c r="AO8" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -1845,12 +1845,12 @@
         <v>8</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
       <c r="N9" s="4"/>
       <c r="T9" s="2" t="s">
         <v>23</v>
@@ -1922,7 +1922,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL9" s="12" t="str">
+      <c r="AL9" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -1934,7 +1934,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO9" s="12" t="str">
+      <c r="AO9" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -1963,10 +1963,10 @@
         <v>Math</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
       <c r="N10" s="4"/>
       <c r="V10" s="9" t="str">
         <f t="shared" si="3"/>
@@ -2032,7 +2032,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL10" s="12" t="str">
+      <c r="AL10" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -2044,7 +2044,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO10" s="12" t="str">
+      <c r="AO10" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -2081,16 +2081,16 @@
       <c r="I11" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="L11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="10" t="s">
         <v>33</v>
       </c>
       <c r="N11" s="4" t="s">
@@ -2166,7 +2166,7 @@
         <f t="shared" si="17"/>
         <v>, scalar</v>
       </c>
-      <c r="AL11" s="12" t="str">
+      <c r="AL11" s="11" t="str">
         <f t="shared" si="18"/>
         <v>, scalar</v>
       </c>
@@ -2178,7 +2178,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO11" s="12" t="str">
+      <c r="AO11" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -2207,10 +2207,10 @@
         <v>Misc</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
       <c r="N12" s="4"/>
       <c r="V12" s="9" t="str">
         <f t="shared" si="3"/>
@@ -2276,7 +2276,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL12" s="12" t="str">
+      <c r="AL12" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -2288,7 +2288,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO12" s="12" t="str">
+      <c r="AO12" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -2317,12 +2317,12 @@
         <v>8</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
       <c r="N13" s="4" t="s">
         <v>10</v>
       </c>
@@ -2396,7 +2396,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL13" s="12" t="str">
+      <c r="AL13" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -2408,7 +2408,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO13" s="12" t="str">
+      <c r="AO13" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -2437,10 +2437,10 @@
         <v>I/O</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
       <c r="N14" s="4"/>
       <c r="V14" s="9" t="str">
         <f t="shared" si="3"/>
@@ -2506,7 +2506,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL14" s="12" t="str">
+      <c r="AL14" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -2518,7 +2518,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO14" s="12" t="str">
+      <c r="AO14" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -2544,10 +2544,10 @@
         <v>scalar</v>
       </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
       <c r="N15" s="4"/>
       <c r="V15" s="9" t="str">
         <f t="shared" si="3"/>
@@ -2613,7 +2613,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL15" s="12" t="str">
+      <c r="AL15" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -2625,7 +2625,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO15" s="12" t="str">
+      <c r="AO15" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -2651,10 +2651,10 @@
         <v>34</v>
       </c>
       <c r="I16" s="3"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
       <c r="N16" s="4" t="s">
         <v>10</v>
       </c>
@@ -2731,7 +2731,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL16" s="12" t="str">
+      <c r="AL16" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -2743,7 +2743,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO16" s="12" t="str">
+      <c r="AO16" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -2772,10 +2772,10 @@
         <v>37</v>
       </c>
       <c r="I17" s="3"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
       <c r="N17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2852,7 +2852,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL17" s="12" t="str">
+      <c r="AL17" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -2864,7 +2864,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO17" s="12" t="str">
+      <c r="AO17" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -2893,10 +2893,10 @@
         <v>40</v>
       </c>
       <c r="I18" s="3"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
       <c r="N18" s="4" t="s">
         <v>10</v>
       </c>
@@ -2973,7 +2973,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL18" s="12" t="str">
+      <c r="AL18" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -2985,7 +2985,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO18" s="12" t="str">
+      <c r="AO18" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -3014,10 +3014,10 @@
         <v>sound</v>
       </c>
       <c r="I19" s="3"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
       <c r="N19" s="4"/>
       <c r="V19" s="9" t="str">
         <f t="shared" si="3"/>
@@ -3083,7 +3083,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL19" s="12" t="str">
+      <c r="AL19" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -3095,7 +3095,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO19" s="12" t="str">
+      <c r="AO19" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -3121,10 +3121,10 @@
         <v>44</v>
       </c>
       <c r="I20" s="3"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
       <c r="N20" s="4" t="s">
         <v>10</v>
       </c>
@@ -3198,7 +3198,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL20" s="12" t="str">
+      <c r="AL20" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -3210,7 +3210,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO20" s="12" t="str">
+      <c r="AO20" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -3242,12 +3242,12 @@
         <v>8</v>
       </c>
       <c r="I21" s="3"/>
-      <c r="J21" s="11" t="s">
+      <c r="J21" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
       <c r="N21" s="4"/>
       <c r="T21" s="2" t="s">
         <v>47</v>
@@ -3319,7 +3319,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL21" s="12" t="str">
+      <c r="AL21" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -3331,7 +3331,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO21" s="12" t="str">
+      <c r="AO21" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -3360,10 +3360,10 @@
         <v>imaging</v>
       </c>
       <c r="I22" s="3"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
       <c r="N22" s="4"/>
       <c r="V22" s="9" t="str">
         <f t="shared" si="3"/>
@@ -3429,7 +3429,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL22" s="12" t="str">
+      <c r="AL22" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -3441,7 +3441,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO22" s="12" t="str">
+      <c r="AO22" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -3467,10 +3467,10 @@
         <v>50</v>
       </c>
       <c r="I23" s="3"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
       <c r="N23" s="4" t="s">
         <v>10</v>
       </c>
@@ -3553,7 +3553,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL23" s="12" t="str">
+      <c r="AL23" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -3565,7 +3565,7 @@
         <f t="shared" si="20"/>
         <v>, intrinsics</v>
       </c>
-      <c r="AO23" s="12" t="str">
+      <c r="AO23" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -3600,14 +3600,14 @@
         <v>55</v>
       </c>
       <c r="I24" s="3"/>
-      <c r="J24" s="11" t="s">
+      <c r="J24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K24" s="11" t="s">
+      <c r="K24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
       <c r="N24" s="4" t="s">
         <v>56</v>
       </c>
@@ -3681,7 +3681,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL24" s="12" t="str">
+      <c r="AL24" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -3693,7 +3693,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO24" s="12" t="str">
+      <c r="AO24" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -3722,10 +3722,10 @@
         <v>59</v>
       </c>
       <c r="I25" s="3"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
       <c r="N25" s="4" t="s">
         <v>10</v>
       </c>
@@ -3802,7 +3802,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL25" s="12" t="str">
+      <c r="AL25" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -3814,7 +3814,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO25" s="12" t="str">
+      <c r="AO25" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -3849,14 +3849,14 @@
         <v>65</v>
       </c>
       <c r="I26" s="3"/>
-      <c r="J26" s="11" t="s">
+      <c r="J26" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="K26" s="11" t="s">
+      <c r="K26" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
       <c r="N26" s="4"/>
       <c r="T26" s="2" t="s">
         <v>154</v>
@@ -3928,7 +3928,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL26" s="12" t="str">
+      <c r="AL26" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -3940,7 +3940,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO26" s="12" t="str">
+      <c r="AO26" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -3972,12 +3972,12 @@
         <v>8</v>
       </c>
       <c r="I27" s="3"/>
-      <c r="J27" s="11" t="s">
+      <c r="J27" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
       <c r="N27" s="4"/>
       <c r="T27" s="2" t="s">
         <v>68</v>
@@ -4049,7 +4049,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL27" s="12" t="str">
+      <c r="AL27" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -4061,7 +4061,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO27" s="12" t="str">
+      <c r="AO27" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -4090,10 +4090,10 @@
         <v>155</v>
       </c>
       <c r="I28" s="3"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
       <c r="N28" s="4" t="s">
         <v>10</v>
       </c>
@@ -4170,7 +4170,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL28" s="12" t="str">
+      <c r="AL28" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -4182,7 +4182,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO28" s="12" t="str">
+      <c r="AO28" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -4214,12 +4214,12 @@
         <v>8</v>
       </c>
       <c r="I29" s="3"/>
-      <c r="J29" s="11" t="s">
+      <c r="J29" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
       <c r="N29" s="4"/>
       <c r="T29" s="2" t="s">
         <v>72</v>
@@ -4291,7 +4291,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL29" s="12" t="str">
+      <c r="AL29" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -4303,7 +4303,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO29" s="12" t="str">
+      <c r="AO29" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -4332,10 +4332,10 @@
         <v>74</v>
       </c>
       <c r="I30" s="3"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
       <c r="N30" s="4" t="s">
         <v>10</v>
       </c>
@@ -4412,7 +4412,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL30" s="12" t="str">
+      <c r="AL30" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -4424,7 +4424,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO30" s="12" t="str">
+      <c r="AO30" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -4453,10 +4453,10 @@
         <v>body</v>
       </c>
       <c r="I31" s="3"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
       <c r="N31" s="4"/>
       <c r="V31" s="9" t="str">
         <f t="shared" si="3"/>
@@ -4522,7 +4522,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL31" s="12" t="str">
+      <c r="AL31" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -4534,7 +4534,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO31" s="12" t="str">
+      <c r="AO31" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -4560,10 +4560,10 @@
         <v>77</v>
       </c>
       <c r="I32" s="3"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
       <c r="N32" s="4" t="s">
         <v>10</v>
       </c>
@@ -4640,7 +4640,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL32" s="12" t="str">
+      <c r="AL32" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -4652,7 +4652,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO32" s="12" t="str">
+      <c r="AO32" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -4681,10 +4681,10 @@
         <v>80</v>
       </c>
       <c r="I33" s="3"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
       <c r="N33" s="4" t="s">
         <v>10</v>
       </c>
@@ -4758,7 +4758,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL33" s="12" t="str">
+      <c r="AL33" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -4770,7 +4770,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO33" s="12" t="str">
+      <c r="AO33" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -4799,10 +4799,10 @@
         <v>82</v>
       </c>
       <c r="I34" s="3"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
       <c r="N34" s="4" t="s">
         <v>10</v>
       </c>
@@ -4876,7 +4876,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL34" s="12" t="str">
+      <c r="AL34" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -4888,7 +4888,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO34" s="12" t="str">
+      <c r="AO34" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -4923,14 +4923,14 @@
         <v>85</v>
       </c>
       <c r="I35" s="3"/>
-      <c r="J35" s="11" t="s">
+      <c r="J35" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="K35" s="11" t="s">
+      <c r="K35" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
       <c r="N35" s="4"/>
       <c r="T35" s="2" t="s">
         <v>86</v>
@@ -4999,7 +4999,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL35" s="12" t="str">
+      <c r="AL35" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -5011,7 +5011,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO35" s="12" t="str">
+      <c r="AO35" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -5046,14 +5046,14 @@
         <v>85</v>
       </c>
       <c r="I36" s="3"/>
-      <c r="J36" s="11" t="s">
+      <c r="J36" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="K36" s="11" t="s">
+      <c r="K36" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
       <c r="N36" s="4"/>
       <c r="T36" s="2" t="s">
         <v>88</v>
@@ -5122,7 +5122,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL36" s="12" t="str">
+      <c r="AL36" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -5134,7 +5134,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO36" s="12" t="str">
+      <c r="AO36" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -5163,10 +5163,10 @@
         <v>CV</v>
       </c>
       <c r="I37" s="3"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
       <c r="N37" s="4"/>
       <c r="V37" s="9" t="str">
         <f t="shared" si="3"/>
@@ -5232,7 +5232,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL37" s="12" t="str">
+      <c r="AL37" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -5244,7 +5244,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO37" s="12" t="str">
+      <c r="AO37" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -5270,10 +5270,10 @@
         <v>Image Processing</v>
       </c>
       <c r="I38" s="3"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
       <c r="N38" s="4"/>
       <c r="V38" s="9" t="str">
         <f t="shared" si="3"/>
@@ -5339,7 +5339,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL38" s="12" t="str">
+      <c r="AL38" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -5351,7 +5351,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO38" s="12" t="str">
+      <c r="AO38" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -5377,10 +5377,10 @@
         <v>91</v>
       </c>
       <c r="I39" s="3"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
       <c r="N39" s="4" t="s">
         <v>10</v>
       </c>
@@ -5454,7 +5454,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL39" s="12" t="str">
+      <c r="AL39" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -5466,7 +5466,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO39" s="12" t="str">
+      <c r="AO39" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -5495,10 +5495,10 @@
         <v>93</v>
       </c>
       <c r="I40" s="3"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
       <c r="N40" s="4" t="s">
         <v>10</v>
       </c>
@@ -5572,7 +5572,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL40" s="12" t="str">
+      <c r="AL40" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -5584,7 +5584,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO40" s="12" t="str">
+      <c r="AO40" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -5619,14 +5619,14 @@
         <v>96</v>
       </c>
       <c r="I41" s="3"/>
-      <c r="J41" s="11" t="s">
+      <c r="J41" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="K41" s="11" t="s">
+      <c r="K41" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
       <c r="N41" s="4" t="s">
         <v>10</v>
       </c>
@@ -5700,7 +5700,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL41" s="12" t="str">
+      <c r="AL41" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -5712,7 +5712,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO41" s="12" t="str">
+      <c r="AO41" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -5744,12 +5744,12 @@
         <v>8</v>
       </c>
       <c r="I42" s="3"/>
-      <c r="J42" s="11" t="s">
+      <c r="J42" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
       <c r="N42" s="4" t="s">
         <v>10</v>
       </c>
@@ -5823,7 +5823,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL42" s="12" t="str">
+      <c r="AL42" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -5835,7 +5835,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO42" s="12" t="str">
+      <c r="AO42" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -5867,12 +5867,12 @@
         <v>8</v>
       </c>
       <c r="I43" s="3"/>
-      <c r="J43" s="11" t="s">
+      <c r="J43" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
       <c r="N43" s="4" t="s">
         <v>10</v>
       </c>
@@ -5946,7 +5946,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL43" s="12" t="str">
+      <c r="AL43" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -5958,7 +5958,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO43" s="12" t="str">
+      <c r="AO43" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -5987,12 +5987,12 @@
         <v>8</v>
       </c>
       <c r="I44" s="3"/>
-      <c r="J44" s="11" t="s">
+      <c r="J44" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
       <c r="N44" s="4" t="s">
         <v>10</v>
       </c>
@@ -6066,7 +6066,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL44" s="12" t="str">
+      <c r="AL44" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -6078,7 +6078,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO44" s="12" t="str">
+      <c r="AO44" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -6115,16 +6115,16 @@
       <c r="I45" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J45" s="11" t="s">
+      <c r="J45" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="K45" s="11" t="s">
+      <c r="K45" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="L45" s="11" t="s">
+      <c r="L45" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="M45" s="11" t="s">
+      <c r="M45" s="10" t="s">
         <v>98</v>
       </c>
       <c r="N45" s="4" t="s">
@@ -6200,7 +6200,7 @@
         <f t="shared" si="17"/>
         <v>, gray</v>
       </c>
-      <c r="AL45" s="12" t="str">
+      <c r="AL45" s="11" t="str">
         <f t="shared" si="18"/>
         <v>, gray</v>
       </c>
@@ -6212,7 +6212,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO45" s="12" t="str">
+      <c r="AO45" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -6241,12 +6241,12 @@
         <v>8</v>
       </c>
       <c r="I46" s="3"/>
-      <c r="J46" s="11" t="s">
+      <c r="J46" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
       <c r="N46" s="4" t="s">
         <v>105</v>
       </c>
@@ -6332,7 +6332,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL46" s="12" t="str">
+      <c r="AL46" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -6344,7 +6344,7 @@
         <f t="shared" si="20"/>
         <v>, gray</v>
       </c>
-      <c r="AO46" s="12" t="str">
+      <c r="AO46" s="11" t="str">
         <f t="shared" si="21"/>
         <v>, gray</v>
       </c>
@@ -6376,14 +6376,14 @@
         <v>112</v>
       </c>
       <c r="I47" s="3"/>
-      <c r="J47" s="11" t="s">
+      <c r="J47" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="K47" s="11" t="s">
+      <c r="K47" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
       <c r="N47" s="4" t="s">
         <v>10</v>
       </c>
@@ -6460,7 +6460,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL47" s="12" t="str">
+      <c r="AL47" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -6472,7 +6472,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO47" s="12" t="str">
+      <c r="AO47" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -6507,16 +6507,16 @@
         <v>117</v>
       </c>
       <c r="I48" s="3"/>
-      <c r="J48" s="11" t="s">
+      <c r="J48" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="K48" s="11" t="s">
+      <c r="K48" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="L48" s="11" t="s">
+      <c r="L48" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="M48" s="11"/>
+      <c r="M48" s="10"/>
       <c r="N48" s="4" t="s">
         <v>10</v>
       </c>
@@ -6590,7 +6590,7 @@
         <f t="shared" si="17"/>
         <v>, int</v>
       </c>
-      <c r="AL48" s="12" t="str">
+      <c r="AL48" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -6602,7 +6602,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO48" s="12" t="str">
+      <c r="AO48" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -6637,16 +6637,16 @@
         <v>85</v>
       </c>
       <c r="I49" s="3"/>
-      <c r="J49" s="11" t="s">
+      <c r="J49" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="K49" s="11" t="s">
+      <c r="K49" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="L49" s="11" t="s">
+      <c r="L49" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="M49" s="11"/>
+      <c r="M49" s="10"/>
       <c r="N49" s="4" t="s">
         <v>10</v>
       </c>
@@ -6720,7 +6720,7 @@
         <f t="shared" si="17"/>
         <v>, gray</v>
       </c>
-      <c r="AL49" s="12" t="str">
+      <c r="AL49" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -6732,7 +6732,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO49" s="12" t="str">
+      <c r="AO49" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -6764,14 +6764,14 @@
         <v>122</v>
       </c>
       <c r="I50" s="3"/>
-      <c r="J50" s="11" t="s">
+      <c r="J50" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="K50" s="11" t="s">
+      <c r="K50" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="L50" s="11"/>
-      <c r="M50" s="11"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
       <c r="N50" s="4" t="s">
         <v>10</v>
       </c>
@@ -6842,7 +6842,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL50" s="12" t="str">
+      <c r="AL50" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -6854,7 +6854,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO50" s="12" t="str">
+      <c r="AO50" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -6880,10 +6880,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I51" s="3"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
       <c r="N51" s="4"/>
       <c r="V51" s="9" t="str">
         <f t="shared" si="3"/>
@@ -6949,7 +6949,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL51" s="12" t="str">
+      <c r="AL51" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -6961,7 +6961,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO51" s="12" t="str">
+      <c r="AO51" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -6990,12 +6990,12 @@
         <v>8</v>
       </c>
       <c r="I52" s="3"/>
-      <c r="J52" s="11" t="s">
+      <c r="J52" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="K52" s="11"/>
-      <c r="L52" s="11"/>
-      <c r="M52" s="11"/>
+      <c r="K52" s="10"/>
+      <c r="L52" s="10"/>
+      <c r="M52" s="10"/>
       <c r="N52" s="4" t="s">
         <v>10</v>
       </c>
@@ -7069,7 +7069,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL52" s="12" t="str">
+      <c r="AL52" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -7081,7 +7081,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO52" s="12" t="str">
+      <c r="AO52" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -7189,7 +7189,7 @@
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="AL53" s="12" t="str">
+      <c r="AL53" s="11" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
@@ -7201,7 +7201,7 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="AO53" s="12" t="str">
+      <c r="AO53" s="11" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -7224,10 +7224,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I54" s="3"/>
-      <c r="J54" s="11"/>
-      <c r="K54" s="11"/>
-      <c r="L54" s="11"/>
-      <c r="M54" s="11"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+      <c r="L54" s="10"/>
+      <c r="M54" s="10"/>
       <c r="N54" s="4"/>
       <c r="V54" s="9" t="str">
         <f t="shared" ref="V54:V99" si="34">"["&amp;IF(RIGHT(F54,5)="(opt)","optional('"&amp;LEFT(F54,LEN(F54)-5)&amp;"')",IF(ISBLANK(F54),"","required('"&amp;F54&amp;"')"))</f>
@@ -7280,10 +7280,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I55" s="3"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
-      <c r="L55" s="11"/>
-      <c r="M55" s="11"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10"/>
+      <c r="L55" s="10"/>
+      <c r="M55" s="10"/>
       <c r="N55" s="4"/>
       <c r="V55" s="9" t="str">
         <f t="shared" si="34"/>
@@ -7336,10 +7336,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I56" s="3"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="11"/>
-      <c r="L56" s="11"/>
-      <c r="M56" s="11"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="10"/>
+      <c r="L56" s="10"/>
+      <c r="M56" s="10"/>
       <c r="N56" s="4"/>
       <c r="V56" s="9" t="str">
         <f t="shared" si="34"/>
@@ -7392,10 +7392,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I57" s="3"/>
-      <c r="J57" s="11"/>
-      <c r="K57" s="11"/>
-      <c r="L57" s="11"/>
-      <c r="M57" s="11"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
+      <c r="L57" s="10"/>
+      <c r="M57" s="10"/>
       <c r="N57" s="4"/>
       <c r="V57" s="9" t="str">
         <f t="shared" si="34"/>
@@ -7448,10 +7448,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I58" s="3"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-      <c r="L58" s="11"/>
-      <c r="M58" s="11"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="10"/>
+      <c r="L58" s="10"/>
+      <c r="M58" s="10"/>
       <c r="N58" s="4"/>
       <c r="V58" s="9" t="str">
         <f t="shared" si="34"/>
@@ -7504,10 +7504,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I59" s="3"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="11"/>
-      <c r="L59" s="11"/>
-      <c r="M59" s="11"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
+      <c r="M59" s="10"/>
       <c r="N59" s="4"/>
       <c r="V59" s="9" t="str">
         <f t="shared" si="34"/>
@@ -7560,10 +7560,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I60" s="3"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
-      <c r="L60" s="11"/>
-      <c r="M60" s="11"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
+      <c r="L60" s="10"/>
+      <c r="M60" s="10"/>
       <c r="N60" s="4"/>
       <c r="V60" s="9" t="str">
         <f t="shared" si="34"/>
@@ -7616,10 +7616,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I61" s="3"/>
-      <c r="J61" s="11"/>
-      <c r="K61" s="11"/>
-      <c r="L61" s="11"/>
-      <c r="M61" s="11"/>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10"/>
+      <c r="L61" s="10"/>
+      <c r="M61" s="10"/>
       <c r="N61" s="4"/>
       <c r="V61" s="9" t="str">
         <f t="shared" si="34"/>
@@ -7672,10 +7672,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I62" s="3"/>
-      <c r="J62" s="11"/>
-      <c r="K62" s="11"/>
-      <c r="L62" s="11"/>
-      <c r="M62" s="11"/>
+      <c r="J62" s="10"/>
+      <c r="K62" s="10"/>
+      <c r="L62" s="10"/>
+      <c r="M62" s="10"/>
       <c r="N62" s="4"/>
       <c r="V62" s="9" t="str">
         <f t="shared" si="34"/>
@@ -7728,10 +7728,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I63" s="3"/>
-      <c r="J63" s="11"/>
-      <c r="K63" s="11"/>
-      <c r="L63" s="11"/>
-      <c r="M63" s="11"/>
+      <c r="J63" s="10"/>
+      <c r="K63" s="10"/>
+      <c r="L63" s="10"/>
+      <c r="M63" s="10"/>
       <c r="N63" s="4"/>
       <c r="V63" s="9" t="str">
         <f t="shared" si="34"/>
@@ -7784,10 +7784,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I64" s="3"/>
-      <c r="J64" s="11"/>
-      <c r="K64" s="11"/>
-      <c r="L64" s="11"/>
-      <c r="M64" s="11"/>
+      <c r="J64" s="10"/>
+      <c r="K64" s="10"/>
+      <c r="L64" s="10"/>
+      <c r="M64" s="10"/>
       <c r="N64" s="4"/>
       <c r="V64" s="9" t="str">
         <f t="shared" si="34"/>
@@ -7840,10 +7840,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I65" s="3"/>
-      <c r="J65" s="11"/>
-      <c r="K65" s="11"/>
-      <c r="L65" s="11"/>
-      <c r="M65" s="11"/>
+      <c r="J65" s="10"/>
+      <c r="K65" s="10"/>
+      <c r="L65" s="10"/>
+      <c r="M65" s="10"/>
       <c r="N65" s="4"/>
       <c r="V65" s="9" t="str">
         <f t="shared" si="34"/>
@@ -7896,10 +7896,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I66" s="3"/>
-      <c r="J66" s="11"/>
-      <c r="K66" s="11"/>
-      <c r="L66" s="11"/>
-      <c r="M66" s="11"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="10"/>
+      <c r="L66" s="10"/>
+      <c r="M66" s="10"/>
       <c r="N66" s="4"/>
       <c r="V66" s="9" t="str">
         <f t="shared" si="34"/>
@@ -7952,10 +7952,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I67" s="3"/>
-      <c r="J67" s="11"/>
-      <c r="K67" s="11"/>
-      <c r="L67" s="11"/>
-      <c r="M67" s="11"/>
+      <c r="J67" s="10"/>
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="10"/>
       <c r="N67" s="4"/>
       <c r="V67" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8008,10 +8008,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I68" s="3"/>
-      <c r="J68" s="11"/>
-      <c r="K68" s="11"/>
-      <c r="L68" s="11"/>
-      <c r="M68" s="11"/>
+      <c r="J68" s="10"/>
+      <c r="K68" s="10"/>
+      <c r="L68" s="10"/>
+      <c r="M68" s="10"/>
       <c r="N68" s="4"/>
       <c r="V68" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8064,10 +8064,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I69" s="3"/>
-      <c r="J69" s="11"/>
-      <c r="K69" s="11"/>
-      <c r="L69" s="11"/>
-      <c r="M69" s="11"/>
+      <c r="J69" s="10"/>
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="10"/>
       <c r="N69" s="4"/>
       <c r="V69" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8120,10 +8120,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I70" s="3"/>
-      <c r="J70" s="11"/>
-      <c r="K70" s="11"/>
-      <c r="L70" s="11"/>
-      <c r="M70" s="11"/>
+      <c r="J70" s="10"/>
+      <c r="K70" s="10"/>
+      <c r="L70" s="10"/>
+      <c r="M70" s="10"/>
       <c r="N70" s="4"/>
       <c r="V70" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8176,10 +8176,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I71" s="3"/>
-      <c r="J71" s="11"/>
-      <c r="K71" s="11"/>
-      <c r="L71" s="11"/>
-      <c r="M71" s="11"/>
+      <c r="J71" s="10"/>
+      <c r="K71" s="10"/>
+      <c r="L71" s="10"/>
+      <c r="M71" s="10"/>
       <c r="N71" s="4"/>
       <c r="V71" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8232,10 +8232,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I72" s="3"/>
-      <c r="J72" s="11"/>
-      <c r="K72" s="11"/>
-      <c r="L72" s="11"/>
-      <c r="M72" s="11"/>
+      <c r="J72" s="10"/>
+      <c r="K72" s="10"/>
+      <c r="L72" s="10"/>
+      <c r="M72" s="10"/>
       <c r="N72" s="4"/>
       <c r="V72" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8288,10 +8288,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I73" s="3"/>
-      <c r="J73" s="11"/>
-      <c r="K73" s="11"/>
-      <c r="L73" s="11"/>
-      <c r="M73" s="11"/>
+      <c r="J73" s="10"/>
+      <c r="K73" s="10"/>
+      <c r="L73" s="10"/>
+      <c r="M73" s="10"/>
       <c r="N73" s="4"/>
       <c r="V73" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8344,10 +8344,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I74" s="3"/>
-      <c r="J74" s="11"/>
-      <c r="K74" s="11"/>
-      <c r="L74" s="11"/>
-      <c r="M74" s="11"/>
+      <c r="J74" s="10"/>
+      <c r="K74" s="10"/>
+      <c r="L74" s="10"/>
+      <c r="M74" s="10"/>
       <c r="N74" s="4"/>
       <c r="V74" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8400,10 +8400,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I75" s="3"/>
-      <c r="J75" s="11"/>
-      <c r="K75" s="11"/>
-      <c r="L75" s="11"/>
-      <c r="M75" s="11"/>
+      <c r="J75" s="10"/>
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
+      <c r="M75" s="10"/>
       <c r="N75" s="4"/>
       <c r="V75" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8456,10 +8456,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I76" s="3"/>
-      <c r="J76" s="11"/>
-      <c r="K76" s="11"/>
-      <c r="L76" s="11"/>
-      <c r="M76" s="11"/>
+      <c r="J76" s="10"/>
+      <c r="K76" s="10"/>
+      <c r="L76" s="10"/>
+      <c r="M76" s="10"/>
       <c r="N76" s="4"/>
       <c r="V76" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8512,10 +8512,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I77" s="3"/>
-      <c r="J77" s="11"/>
-      <c r="K77" s="11"/>
-      <c r="L77" s="11"/>
-      <c r="M77" s="11"/>
+      <c r="J77" s="10"/>
+      <c r="K77" s="10"/>
+      <c r="L77" s="10"/>
+      <c r="M77" s="10"/>
       <c r="N77" s="4"/>
       <c r="V77" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8568,10 +8568,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I78" s="3"/>
-      <c r="J78" s="11"/>
-      <c r="K78" s="11"/>
-      <c r="L78" s="11"/>
-      <c r="M78" s="11"/>
+      <c r="J78" s="10"/>
+      <c r="K78" s="10"/>
+      <c r="L78" s="10"/>
+      <c r="M78" s="10"/>
       <c r="N78" s="4"/>
       <c r="V78" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8624,10 +8624,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I79" s="3"/>
-      <c r="J79" s="11"/>
-      <c r="K79" s="11"/>
-      <c r="L79" s="11"/>
-      <c r="M79" s="11"/>
+      <c r="J79" s="10"/>
+      <c r="K79" s="10"/>
+      <c r="L79" s="10"/>
+      <c r="M79" s="10"/>
       <c r="N79" s="4"/>
       <c r="V79" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8680,10 +8680,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I80" s="3"/>
-      <c r="J80" s="11"/>
-      <c r="K80" s="11"/>
-      <c r="L80" s="11"/>
-      <c r="M80" s="11"/>
+      <c r="J80" s="10"/>
+      <c r="K80" s="10"/>
+      <c r="L80" s="10"/>
+      <c r="M80" s="10"/>
       <c r="N80" s="4"/>
       <c r="V80" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8736,10 +8736,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I81" s="3"/>
-      <c r="J81" s="11"/>
-      <c r="K81" s="11"/>
-      <c r="L81" s="11"/>
-      <c r="M81" s="11"/>
+      <c r="J81" s="10"/>
+      <c r="K81" s="10"/>
+      <c r="L81" s="10"/>
+      <c r="M81" s="10"/>
       <c r="N81" s="4"/>
       <c r="V81" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8792,10 +8792,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I82" s="3"/>
-      <c r="J82" s="11"/>
-      <c r="K82" s="11"/>
-      <c r="L82" s="11"/>
-      <c r="M82" s="11"/>
+      <c r="J82" s="10"/>
+      <c r="K82" s="10"/>
+      <c r="L82" s="10"/>
+      <c r="M82" s="10"/>
       <c r="N82" s="4"/>
       <c r="V82" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8848,10 +8848,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I83" s="3"/>
-      <c r="J83" s="11"/>
-      <c r="K83" s="11"/>
-      <c r="L83" s="11"/>
-      <c r="M83" s="11"/>
+      <c r="J83" s="10"/>
+      <c r="K83" s="10"/>
+      <c r="L83" s="10"/>
+      <c r="M83" s="10"/>
       <c r="N83" s="4"/>
       <c r="V83" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8904,10 +8904,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I84" s="3"/>
-      <c r="J84" s="11"/>
-      <c r="K84" s="11"/>
-      <c r="L84" s="11"/>
-      <c r="M84" s="11"/>
+      <c r="J84" s="10"/>
+      <c r="K84" s="10"/>
+      <c r="L84" s="10"/>
+      <c r="M84" s="10"/>
       <c r="N84" s="4"/>
       <c r="V84" s="9" t="str">
         <f t="shared" si="34"/>
@@ -8960,10 +8960,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I85" s="3"/>
-      <c r="J85" s="11"/>
-      <c r="K85" s="11"/>
-      <c r="L85" s="11"/>
-      <c r="M85" s="11"/>
+      <c r="J85" s="10"/>
+      <c r="K85" s="10"/>
+      <c r="L85" s="10"/>
+      <c r="M85" s="10"/>
       <c r="N85" s="4"/>
       <c r="V85" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9016,10 +9016,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I86" s="3"/>
-      <c r="J86" s="11"/>
-      <c r="K86" s="11"/>
-      <c r="L86" s="11"/>
-      <c r="M86" s="11"/>
+      <c r="J86" s="10"/>
+      <c r="K86" s="10"/>
+      <c r="L86" s="10"/>
+      <c r="M86" s="10"/>
       <c r="N86" s="4"/>
       <c r="V86" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9072,10 +9072,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I87" s="3"/>
-      <c r="J87" s="11"/>
-      <c r="K87" s="11"/>
-      <c r="L87" s="11"/>
-      <c r="M87" s="11"/>
+      <c r="J87" s="10"/>
+      <c r="K87" s="10"/>
+      <c r="L87" s="10"/>
+      <c r="M87" s="10"/>
       <c r="N87" s="4"/>
       <c r="V87" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9128,10 +9128,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I88" s="3"/>
-      <c r="J88" s="11"/>
-      <c r="K88" s="11"/>
-      <c r="L88" s="11"/>
-      <c r="M88" s="11"/>
+      <c r="J88" s="10"/>
+      <c r="K88" s="10"/>
+      <c r="L88" s="10"/>
+      <c r="M88" s="10"/>
       <c r="N88" s="4"/>
       <c r="V88" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9184,10 +9184,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I89" s="3"/>
-      <c r="J89" s="11"/>
-      <c r="K89" s="11"/>
-      <c r="L89" s="11"/>
-      <c r="M89" s="11"/>
+      <c r="J89" s="10"/>
+      <c r="K89" s="10"/>
+      <c r="L89" s="10"/>
+      <c r="M89" s="10"/>
       <c r="N89" s="4"/>
       <c r="V89" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9240,10 +9240,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I90" s="3"/>
-      <c r="J90" s="11"/>
-      <c r="K90" s="11"/>
-      <c r="L90" s="11"/>
-      <c r="M90" s="11"/>
+      <c r="J90" s="10"/>
+      <c r="K90" s="10"/>
+      <c r="L90" s="10"/>
+      <c r="M90" s="10"/>
       <c r="N90" s="4"/>
       <c r="V90" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9296,10 +9296,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I91" s="3"/>
-      <c r="J91" s="11"/>
-      <c r="K91" s="11"/>
-      <c r="L91" s="11"/>
-      <c r="M91" s="11"/>
+      <c r="J91" s="10"/>
+      <c r="K91" s="10"/>
+      <c r="L91" s="10"/>
+      <c r="M91" s="10"/>
       <c r="N91" s="4"/>
       <c r="V91" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9352,10 +9352,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I92" s="3"/>
-      <c r="J92" s="11"/>
-      <c r="K92" s="11"/>
-      <c r="L92" s="11"/>
-      <c r="M92" s="11"/>
+      <c r="J92" s="10"/>
+      <c r="K92" s="10"/>
+      <c r="L92" s="10"/>
+      <c r="M92" s="10"/>
       <c r="N92" s="4"/>
       <c r="V92" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9408,10 +9408,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I93" s="3"/>
-      <c r="J93" s="11"/>
-      <c r="K93" s="11"/>
-      <c r="L93" s="11"/>
-      <c r="M93" s="11"/>
+      <c r="J93" s="10"/>
+      <c r="K93" s="10"/>
+      <c r="L93" s="10"/>
+      <c r="M93" s="10"/>
       <c r="N93" s="4"/>
       <c r="V93" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9464,10 +9464,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I94" s="3"/>
-      <c r="J94" s="11"/>
-      <c r="K94" s="11"/>
-      <c r="L94" s="11"/>
-      <c r="M94" s="11"/>
+      <c r="J94" s="10"/>
+      <c r="K94" s="10"/>
+      <c r="L94" s="10"/>
+      <c r="M94" s="10"/>
       <c r="N94" s="4"/>
       <c r="V94" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9520,10 +9520,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I95" s="3"/>
-      <c r="J95" s="11"/>
-      <c r="K95" s="11"/>
-      <c r="L95" s="11"/>
-      <c r="M95" s="11"/>
+      <c r="J95" s="10"/>
+      <c r="K95" s="10"/>
+      <c r="L95" s="10"/>
+      <c r="M95" s="10"/>
       <c r="N95" s="4"/>
       <c r="V95" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9576,10 +9576,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I96" s="3"/>
-      <c r="J96" s="11"/>
-      <c r="K96" s="11"/>
-      <c r="L96" s="11"/>
-      <c r="M96" s="11"/>
+      <c r="J96" s="10"/>
+      <c r="K96" s="10"/>
+      <c r="L96" s="10"/>
+      <c r="M96" s="10"/>
       <c r="N96" s="4"/>
       <c r="V96" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9632,10 +9632,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I97" s="3"/>
-      <c r="J97" s="11"/>
-      <c r="K97" s="11"/>
-      <c r="L97" s="11"/>
-      <c r="M97" s="11"/>
+      <c r="J97" s="10"/>
+      <c r="K97" s="10"/>
+      <c r="L97" s="10"/>
+      <c r="M97" s="10"/>
       <c r="N97" s="4"/>
       <c r="V97" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9688,10 +9688,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I98" s="3"/>
-      <c r="J98" s="11"/>
-      <c r="K98" s="11"/>
-      <c r="L98" s="11"/>
-      <c r="M98" s="11"/>
+      <c r="J98" s="10"/>
+      <c r="K98" s="10"/>
+      <c r="L98" s="10"/>
+      <c r="M98" s="10"/>
       <c r="N98" s="4"/>
       <c r="V98" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9744,10 +9744,10 @@
         <v>FrequencyDomain</v>
       </c>
       <c r="I99" s="3"/>
-      <c r="J99" s="11"/>
-      <c r="K99" s="11"/>
-      <c r="L99" s="11"/>
-      <c r="M99" s="11"/>
+      <c r="J99" s="10"/>
+      <c r="K99" s="10"/>
+      <c r="L99" s="10"/>
+      <c r="M99" s="10"/>
       <c r="N99" s="4"/>
       <c r="V99" s="9" t="str">
         <f t="shared" si="34"/>
@@ -9792,66 +9792,66 @@
     </row>
     <row r="100" spans="3:34" x14ac:dyDescent="0.2">
       <c r="I100" s="3"/>
-      <c r="J100" s="11"/>
-      <c r="K100" s="11"/>
-      <c r="L100" s="11"/>
-      <c r="M100" s="11"/>
+      <c r="J100" s="10"/>
+      <c r="K100" s="10"/>
+      <c r="L100" s="10"/>
+      <c r="M100" s="10"/>
       <c r="N100" s="4"/>
     </row>
     <row r="101" spans="3:34" x14ac:dyDescent="0.2">
       <c r="I101" s="3"/>
-      <c r="J101" s="11"/>
-      <c r="K101" s="11"/>
-      <c r="L101" s="11"/>
-      <c r="M101" s="11"/>
+      <c r="J101" s="10"/>
+      <c r="K101" s="10"/>
+      <c r="L101" s="10"/>
+      <c r="M101" s="10"/>
       <c r="N101" s="4"/>
     </row>
     <row r="102" spans="3:34" x14ac:dyDescent="0.2">
       <c r="I102" s="3"/>
-      <c r="J102" s="11"/>
-      <c r="K102" s="11"/>
-      <c r="L102" s="11"/>
-      <c r="M102" s="11"/>
+      <c r="J102" s="10"/>
+      <c r="K102" s="10"/>
+      <c r="L102" s="10"/>
+      <c r="M102" s="10"/>
       <c r="N102" s="4"/>
     </row>
     <row r="103" spans="3:34" x14ac:dyDescent="0.2">
       <c r="I103" s="3"/>
-      <c r="J103" s="11"/>
-      <c r="K103" s="11"/>
-      <c r="L103" s="11"/>
-      <c r="M103" s="11"/>
+      <c r="J103" s="10"/>
+      <c r="K103" s="10"/>
+      <c r="L103" s="10"/>
+      <c r="M103" s="10"/>
       <c r="N103" s="4"/>
     </row>
     <row r="104" spans="3:34" x14ac:dyDescent="0.2">
       <c r="I104" s="3"/>
-      <c r="J104" s="11"/>
-      <c r="K104" s="11"/>
-      <c r="L104" s="11"/>
-      <c r="M104" s="11"/>
+      <c r="J104" s="10"/>
+      <c r="K104" s="10"/>
+      <c r="L104" s="10"/>
+      <c r="M104" s="10"/>
       <c r="N104" s="4"/>
     </row>
     <row r="105" spans="3:34" x14ac:dyDescent="0.2">
       <c r="I105" s="3"/>
-      <c r="J105" s="11"/>
-      <c r="K105" s="11"/>
-      <c r="L105" s="11"/>
-      <c r="M105" s="11"/>
+      <c r="J105" s="10"/>
+      <c r="K105" s="10"/>
+      <c r="L105" s="10"/>
+      <c r="M105" s="10"/>
       <c r="N105" s="4"/>
     </row>
     <row r="106" spans="3:34" x14ac:dyDescent="0.2">
       <c r="I106" s="3"/>
-      <c r="J106" s="11"/>
-      <c r="K106" s="11"/>
-      <c r="L106" s="11"/>
-      <c r="M106" s="11"/>
+      <c r="J106" s="10"/>
+      <c r="K106" s="10"/>
+      <c r="L106" s="10"/>
+      <c r="M106" s="10"/>
       <c r="N106" s="4"/>
     </row>
     <row r="107" spans="3:34" x14ac:dyDescent="0.2">
       <c r="I107" s="3"/>
-      <c r="J107" s="11"/>
-      <c r="K107" s="11"/>
-      <c r="L107" s="11"/>
-      <c r="M107" s="11"/>
+      <c r="J107" s="10"/>
+      <c r="K107" s="10"/>
+      <c r="L107" s="10"/>
+      <c r="M107" s="10"/>
       <c r="N107" s="4"/>
     </row>
   </sheetData>
@@ -9870,7 +9870,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
for some SVN(?) reason that debug y/2 in JVisionEngine keeps coming back. Also working towards working model in Blockflow
</commit_message>
<xml_diff>
--- a/doc/flo/Blocks.xlsx
+++ b/doc/flo/Blocks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="555" windowWidth="12135" windowHeight="8520"/>
+    <workbookView xWindow="270" yWindow="555" windowWidth="12135" windowHeight="8520" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BlockTypes" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="246">
   <si>
     <t>Block Types</t>
   </si>
@@ -730,6 +730,30 @@
   </si>
   <si>
     <t>OC</t>
+  </si>
+  <si>
+    <t>flick pan</t>
+  </si>
+  <si>
+    <t>mouse wheel</t>
+  </si>
+  <si>
+    <t>ctrl space</t>
+  </si>
+  <si>
+    <t>strictly on any drag that exits the main window</t>
+  </si>
+  <si>
+    <t>Right menu</t>
+  </si>
+  <si>
+    <t>extend select</t>
+  </si>
+  <si>
+    <t>drag select</t>
+  </si>
+  <si>
+    <t>all controls show up in a panel, tab or click in panel to focus there</t>
   </si>
 </sst>
 </file>
@@ -1167,7 +1191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <pane xSplit="8985" ySplit="540" topLeftCell="AU24" activePane="bottomRight"/>
       <selection activeCell="AW14" sqref="AW14"/>
       <selection pane="topRight" activeCell="AU1" sqref="AU1"/>
@@ -11732,10 +11756,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11743,226 +11767,264 @@
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="36.140625" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>177</v>
       </c>
       <c r="D2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>211</v>
       </c>
       <c r="D5" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>190</v>
-      </c>
-    </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>182</v>
+      <c r="B20" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>193</v>
+      <c r="A22" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>197</v>
+      <c r="B27" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+    <row r="33" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+    <row r="36" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+      <c r="F36" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
+    <row r="50" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
         <v>216</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Stu's camera changer. More blocks.
</commit_message>
<xml_diff>
--- a/doc/flo/Blocks.xlsx
+++ b/doc/flo/Blocks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="288">
   <si>
     <t>Block Types</t>
   </si>
@@ -832,6 +832,54 @@
   </si>
   <si>
     <t>protocoords</t>
+  </si>
+  <si>
+    <t>blocksheet1_01.png</t>
+  </si>
+  <si>
+    <t>blocksheet1_02.png</t>
+  </si>
+  <si>
+    <t>blocksheet1_03.png</t>
+  </si>
+  <si>
+    <t>blocksheet1_04.png</t>
+  </si>
+  <si>
+    <t>blocksheet1_05.png</t>
+  </si>
+  <si>
+    <t>blocksheet1_06.png</t>
+  </si>
+  <si>
+    <t>blocksheet1_07.png</t>
+  </si>
+  <si>
+    <t>blocksheet1_09.png</t>
+  </si>
+  <si>
+    <t>blocksheet1_13.png</t>
+  </si>
+  <si>
+    <t>blocksheet1_14.png</t>
+  </si>
+  <si>
+    <t>blocksheet1_10.png</t>
+  </si>
+  <si>
+    <t>blocksheet1_15.png</t>
+  </si>
+  <si>
+    <t>blocksheet1_11.png</t>
+  </si>
+  <si>
+    <t>blocksheet1_16.png</t>
+  </si>
+  <si>
+    <t>blocksheet1_17.png</t>
+  </si>
+  <si>
+    <t>blocksheet0-_08.png</t>
   </si>
 </sst>
 </file>
@@ -1289,12 +1337,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane xSplit="8985" ySplit="540" topLeftCell="BC12" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="9000" ySplit="540" topLeftCell="BC1" activePane="bottomRight"/>
       <selection activeCell="AH1" sqref="AH1"/>
       <selection pane="topRight" activeCell="BE1" sqref="BE1"/>
-      <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
-      <selection pane="bottomRight" activeCell="BF11" sqref="BF11"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="BD6" sqref="BD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1808,8 +1856,8 @@
         <v>0</v>
       </c>
       <c r="AH5" t="str">
-        <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== flipflop ===========&lt;&gt;section(flipflop, 'Control').&lt;&gt;subsection(flipflop, 'Control').&lt;&gt;description(flipflop, 'a jk flipflop').&lt;&gt;visual_style(flipflop,  normal).&lt;&gt;inputs(flipflop, [required('J'), required('K')]).&lt;&gt;outputs(flipflop, ['O']).&lt;&gt;input_types(flipflop, [pulse, pulse]).&lt;&gt;output_types(flipflop, [int]).&lt;&gt;</v>
+        <f>IF(ISBLANK(E5),"","&lt;&gt;%  ===== "&amp;E5&amp;" ===========&lt;&gt;"&amp;AE5&amp;").&lt;&gt;inputs("&amp;E5&amp;", "&amp;Z5&amp;").&lt;&gt;outputs("&amp;E5&amp;", "&amp;AD5&amp;").&lt;&gt;input_types("&amp;E5&amp;", "&amp;AP5&amp;").&lt;&gt;output_types("&amp;E5&amp;", "&amp;AQ5&amp;").&lt;&gt;"&amp;IF(OR(ISBLANK(E5),ISBLANK(BB16)),"","image_name("&amp;E5&amp;", '/img/blocks/"&amp;BB16&amp;"').&lt;&gt;"))</f>
+        <v>&lt;&gt;%  ===== flipflop ===========&lt;&gt;section(flipflop, 'Control').&lt;&gt;subsection(flipflop, 'Control').&lt;&gt;description(flipflop, 'a jk flipflop').&lt;&gt;visual_style(flipflop,  normal).&lt;&gt;inputs(flipflop, [required('J'), required('K')]).&lt;&gt;outputs(flipflop, ['O']).&lt;&gt;input_types(flipflop, [pulse, pulse]).&lt;&gt;output_types(flipflop, [int]).&lt;&gt;image_name(flipflop, '/img/blocks/blocksheet1_01.png').&lt;&gt;</v>
       </c>
       <c r="AI5" t="str">
         <f t="shared" si="15"/>
@@ -1852,7 +1900,7 @@
       </c>
       <c r="BE5" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== flipflop ===========&lt;&gt;section(flipflop, 'Control').&lt;&gt;subsection(flipflop, 'Control').&lt;&gt;description(flipflop, 'a jk flipflop').&lt;&gt;visual_style(flipflop,  normal).&lt;&gt;inputs(flipflop, [required('J'), required('K')]).&lt;&gt;outputs(flipflop, ['O']).&lt;&gt;input_types(flipflop, [pulse, pulse]).&lt;&gt;output_types(flipflop, [int]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== flipflop ===========&lt;&gt;section(flipflop, 'Control').&lt;&gt;subsection(flipflop, 'Control').&lt;&gt;description(flipflop, 'a jk flipflop').&lt;&gt;visual_style(flipflop,  normal).&lt;&gt;inputs(flipflop, [required('J'), required('K')]).&lt;&gt;outputs(flipflop, ['O']).&lt;&gt;input_types(flipflop, [pulse, pulse]).&lt;&gt;output_types(flipflop, [int]).&lt;&gt;image_name(flipflop, '/img/blocks/blocksheet1_01.png').&lt;&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3214,7 +3262,7 @@
       </c>
       <c r="AH16" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== pulse ===========&lt;&gt;section(pulse, 'I/O').&lt;&gt;subsection(pulse, 'scalar').&lt;&gt;description(pulse, 'Is 1 on the next frame after mouseup').&lt;&gt;visual_style(pulse,  visual_style2).&lt;&gt;inputs(pulse, []).&lt;&gt;outputs(pulse, ['O']).&lt;&gt;input_types(pulse, []).&lt;&gt;output_types(pulse, [pulse]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== pulse ===========&lt;&gt;section(pulse, 'I/O').&lt;&gt;subsection(pulse, 'scalar').&lt;&gt;description(pulse, 'Is 1 on the next frame after mouseup').&lt;&gt;visual_style(pulse,  visual_style2).&lt;&gt;inputs(pulse, []).&lt;&gt;outputs(pulse, ['O']).&lt;&gt;input_types(pulse, []).&lt;&gt;output_types(pulse, [pulse]).&lt;&gt;image_name(pulse, '/img/blocks/blocksheet1_01.png').&lt;&gt;</v>
       </c>
       <c r="AI16" t="str">
         <f t="shared" si="15"/>
@@ -3255,9 +3303,18 @@
       <c r="AS16">
         <v>1</v>
       </c>
+      <c r="BB16" t="s">
+        <v>272</v>
+      </c>
+      <c r="BC16">
+        <v>21</v>
+      </c>
+      <c r="BD16">
+        <v>0</v>
+      </c>
       <c r="BE16" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== pulse ===========&lt;&gt;section(pulse, 'I/O').&lt;&gt;subsection(pulse, 'scalar').&lt;&gt;description(pulse, 'Is 1 on the next frame after mouseup').&lt;&gt;visual_style(pulse,  visual_style2).&lt;&gt;inputs(pulse, []).&lt;&gt;outputs(pulse, ['O']).&lt;&gt;input_types(pulse, []).&lt;&gt;output_types(pulse, [pulse]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== pulse ===========&lt;&gt;section(pulse, 'I/O').&lt;&gt;subsection(pulse, 'scalar').&lt;&gt;description(pulse, 'Is 1 on the next frame after mouseup').&lt;&gt;visual_style(pulse,  visual_style2).&lt;&gt;inputs(pulse, []).&lt;&gt;outputs(pulse, ['O']).&lt;&gt;input_types(pulse, []).&lt;&gt;output_types(pulse, [pulse]).&lt;&gt;image_name(pulse, '/img/blocks/blocksheet1_01.png').&lt;&gt;prototype_coordinates(pulse, 21, 0).&lt;&gt;</v>
       </c>
     </row>
     <row r="17" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3339,7 +3396,7 @@
       </c>
       <c r="AH17" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== proportion ===========&lt;&gt;section(proportion, 'I/O').&lt;&gt;subsection(proportion, 'scalar').&lt;&gt;description(proportion, 'slider value from 0-1').&lt;&gt;visual_style(proportion,  visual_style3).&lt;&gt;inputs(proportion, []).&lt;&gt;outputs(proportion, ['O']).&lt;&gt;input_types(proportion, []).&lt;&gt;output_types(proportion, [proportion]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== proportion ===========&lt;&gt;section(proportion, 'I/O').&lt;&gt;subsection(proportion, 'scalar').&lt;&gt;description(proportion, 'slider value from 0-1').&lt;&gt;visual_style(proportion,  visual_style3).&lt;&gt;inputs(proportion, []).&lt;&gt;outputs(proportion, ['O']).&lt;&gt;input_types(proportion, []).&lt;&gt;output_types(proportion, [proportion]).&lt;&gt;image_name(proportion, '/img/blocks/blocksheet1_02.png').&lt;&gt;</v>
       </c>
       <c r="AI17" t="str">
         <f t="shared" si="15"/>
@@ -3380,9 +3437,19 @@
       <c r="AS17">
         <v>1</v>
       </c>
+      <c r="BB17" t="s">
+        <v>273</v>
+      </c>
+      <c r="BC17">
+        <v>21</v>
+      </c>
+      <c r="BD17">
+        <f>BD16+1</f>
+        <v>1</v>
+      </c>
       <c r="BE17" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== proportion ===========&lt;&gt;section(proportion, 'I/O').&lt;&gt;subsection(proportion, 'scalar').&lt;&gt;description(proportion, 'slider value from 0-1').&lt;&gt;visual_style(proportion,  visual_style3).&lt;&gt;inputs(proportion, []).&lt;&gt;outputs(proportion, ['O']).&lt;&gt;input_types(proportion, []).&lt;&gt;output_types(proportion, [proportion]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== proportion ===========&lt;&gt;section(proportion, 'I/O').&lt;&gt;subsection(proportion, 'scalar').&lt;&gt;description(proportion, 'slider value from 0-1').&lt;&gt;visual_style(proportion,  visual_style3).&lt;&gt;inputs(proportion, []).&lt;&gt;outputs(proportion, ['O']).&lt;&gt;input_types(proportion, []).&lt;&gt;output_types(proportion, [proportion]).&lt;&gt;image_name(proportion, '/img/blocks/blocksheet1_02.png').&lt;&gt;prototype_coordinates(proportion, 21, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="18" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3464,7 +3531,7 @@
       </c>
       <c r="AH18" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== floatval ===========&lt;&gt;section(floatval, 'I/O').&lt;&gt;subsection(floatval, 'scalar').&lt;&gt;description(floatval, 'float value that varies over -inf to +inf').&lt;&gt;visual_style(floatval,  visual_style4).&lt;&gt;inputs(floatval, []).&lt;&gt;outputs(floatval, ['O']).&lt;&gt;input_types(floatval, []).&lt;&gt;output_types(floatval, [float]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== floatval ===========&lt;&gt;section(floatval, 'I/O').&lt;&gt;subsection(floatval, 'scalar').&lt;&gt;description(floatval, 'float value that varies over -inf to +inf').&lt;&gt;visual_style(floatval,  visual_style4).&lt;&gt;inputs(floatval, []).&lt;&gt;outputs(floatval, ['O']).&lt;&gt;input_types(floatval, []).&lt;&gt;output_types(floatval, [float]).&lt;&gt;image_name(floatval, '/img/blocks/blocksheet1_03.png').&lt;&gt;</v>
       </c>
       <c r="AI18" t="str">
         <f t="shared" si="15"/>
@@ -3505,9 +3572,19 @@
       <c r="AS18">
         <v>1</v>
       </c>
+      <c r="BB18" t="s">
+        <v>274</v>
+      </c>
+      <c r="BC18">
+        <v>21</v>
+      </c>
+      <c r="BD18">
+        <f>BD17+1</f>
+        <v>2</v>
+      </c>
       <c r="BE18" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== floatval ===========&lt;&gt;section(floatval, 'I/O').&lt;&gt;subsection(floatval, 'scalar').&lt;&gt;description(floatval, 'float value that varies over -inf to +inf').&lt;&gt;visual_style(floatval,  visual_style4).&lt;&gt;inputs(floatval, []).&lt;&gt;outputs(floatval, ['O']).&lt;&gt;input_types(floatval, []).&lt;&gt;output_types(floatval, [float]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== floatval ===========&lt;&gt;section(floatval, 'I/O').&lt;&gt;subsection(floatval, 'scalar').&lt;&gt;description(floatval, 'float value that varies over -inf to +inf').&lt;&gt;visual_style(floatval,  visual_style4).&lt;&gt;inputs(floatval, []).&lt;&gt;outputs(floatval, ['O']).&lt;&gt;input_types(floatval, []).&lt;&gt;output_types(floatval, [float]).&lt;&gt;image_name(floatval, '/img/blocks/blocksheet1_03.png').&lt;&gt;prototype_coordinates(floatval, 21, 2).&lt;&gt;</v>
       </c>
     </row>
     <row r="19" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3697,7 +3774,7 @@
       </c>
       <c r="AH20" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== mic ===========&lt;&gt;section(mic, 'I/O').&lt;&gt;subsection(mic, 'sound').&lt;&gt;description(mic, 'samples from mic').&lt;&gt;visual_style(mic,  normal).&lt;&gt;inputs(mic, []).&lt;&gt;outputs(mic, ['O']).&lt;&gt;input_types(mic, []).&lt;&gt;output_types(mic, [sample]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== mic ===========&lt;&gt;section(mic, 'I/O').&lt;&gt;subsection(mic, 'sound').&lt;&gt;description(mic, 'samples from mic').&lt;&gt;visual_style(mic,  normal).&lt;&gt;inputs(mic, []).&lt;&gt;outputs(mic, ['O']).&lt;&gt;input_types(mic, []).&lt;&gt;output_types(mic, [sample]).&lt;&gt;image_name(mic, '/img/blocks/blocksheet1_04.png').&lt;&gt;</v>
       </c>
       <c r="AI20" t="str">
         <f t="shared" si="15"/>
@@ -3738,9 +3815,18 @@
       <c r="AS20">
         <v>1</v>
       </c>
+      <c r="BB20" t="s">
+        <v>275</v>
+      </c>
+      <c r="BC20">
+        <v>21</v>
+      </c>
+      <c r="BD20">
+        <v>3</v>
+      </c>
       <c r="BE20" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== mic ===========&lt;&gt;section(mic, 'I/O').&lt;&gt;subsection(mic, 'sound').&lt;&gt;description(mic, 'samples from mic').&lt;&gt;visual_style(mic,  normal).&lt;&gt;inputs(mic, []).&lt;&gt;outputs(mic, ['O']).&lt;&gt;input_types(mic, []).&lt;&gt;output_types(mic, [sample]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== mic ===========&lt;&gt;section(mic, 'I/O').&lt;&gt;subsection(mic, 'sound').&lt;&gt;description(mic, 'samples from mic').&lt;&gt;visual_style(mic,  normal).&lt;&gt;inputs(mic, []).&lt;&gt;outputs(mic, ['O']).&lt;&gt;input_types(mic, []).&lt;&gt;output_types(mic, [sample]).&lt;&gt;image_name(mic, '/img/blocks/blocksheet1_04.png').&lt;&gt;prototype_coordinates(mic, 21, 3).&lt;&gt;</v>
       </c>
     </row>
     <row r="21" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3822,7 +3908,7 @@
       </c>
       <c r="AH21" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== listen ===========&lt;&gt;section(listen, 'I/O').&lt;&gt;subsection(listen, 'sound').&lt;&gt;description(listen, 'Sends sound to default output').&lt;&gt;visual_style(listen,  visual_style5).&lt;&gt;inputs(listen, [required('A')]).&lt;&gt;outputs(listen, []).&lt;&gt;input_types(listen, [sample]).&lt;&gt;output_types(listen, []).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== listen ===========&lt;&gt;section(listen, 'I/O').&lt;&gt;subsection(listen, 'sound').&lt;&gt;description(listen, 'Sends sound to default output').&lt;&gt;visual_style(listen,  visual_style5).&lt;&gt;inputs(listen, [required('A')]).&lt;&gt;outputs(listen, []).&lt;&gt;input_types(listen, [sample]).&lt;&gt;output_types(listen, []).&lt;&gt;image_name(listen, '/img/blocks/blocksheet1_05.png').&lt;&gt;</v>
       </c>
       <c r="AI21" t="str">
         <f t="shared" si="15"/>
@@ -3863,9 +3949,18 @@
       <c r="AS21">
         <v>1</v>
       </c>
+      <c r="BB21" t="s">
+        <v>276</v>
+      </c>
+      <c r="BC21">
+        <v>21</v>
+      </c>
+      <c r="BD21">
+        <v>4</v>
+      </c>
       <c r="BE21" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== listen ===========&lt;&gt;section(listen, 'I/O').&lt;&gt;subsection(listen, 'sound').&lt;&gt;description(listen, 'Sends sound to default output').&lt;&gt;visual_style(listen,  visual_style5).&lt;&gt;inputs(listen, [required('A')]).&lt;&gt;outputs(listen, []).&lt;&gt;input_types(listen, [sample]).&lt;&gt;output_types(listen, []).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== listen ===========&lt;&gt;section(listen, 'I/O').&lt;&gt;subsection(listen, 'sound').&lt;&gt;description(listen, 'Sends sound to default output').&lt;&gt;visual_style(listen,  visual_style5).&lt;&gt;inputs(listen, [required('A')]).&lt;&gt;outputs(listen, []).&lt;&gt;input_types(listen, [sample]).&lt;&gt;output_types(listen, []).&lt;&gt;image_name(listen, '/img/blocks/blocksheet1_05.png').&lt;&gt;prototype_coordinates(listen, 21, 4).&lt;&gt;</v>
       </c>
     </row>
     <row r="22" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4064,7 +4159,7 @@
       </c>
       <c r="AH23" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== camera ===========&lt;&gt;section(camera, 'I/O').&lt;&gt;subsection(camera, 'imaging').&lt;&gt;description(camera, 'O is frames out of camera, K is camera intrinsics').&lt;&gt;visual_style(camera,  visual_style6).&lt;&gt;inputs(camera, []).&lt;&gt;outputs(camera, ['O', 'K']).&lt;&gt;input_types(camera, []).&lt;&gt;output_types(camera, [rgb, intrinsics]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== camera ===========&lt;&gt;section(camera, 'I/O').&lt;&gt;subsection(camera, 'imaging').&lt;&gt;description(camera, 'O is frames out of camera, K is camera intrinsics').&lt;&gt;visual_style(camera,  visual_style6).&lt;&gt;inputs(camera, []).&lt;&gt;outputs(camera, ['O', 'K']).&lt;&gt;input_types(camera, []).&lt;&gt;output_types(camera, [rgb, intrinsics]).&lt;&gt;image_name(camera, '/img/blocks/blocksheet1_06.png').&lt;&gt;</v>
       </c>
       <c r="AI23" t="str">
         <f t="shared" si="15"/>
@@ -4105,9 +4200,18 @@
       <c r="AS23">
         <v>1</v>
       </c>
+      <c r="BB23" t="s">
+        <v>277</v>
+      </c>
+      <c r="BC23">
+        <v>21</v>
+      </c>
+      <c r="BD23">
+        <v>5</v>
+      </c>
       <c r="BE23" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== camera ===========&lt;&gt;section(camera, 'I/O').&lt;&gt;subsection(camera, 'imaging').&lt;&gt;description(camera, 'O is frames out of camera, K is camera intrinsics').&lt;&gt;visual_style(camera,  visual_style6).&lt;&gt;inputs(camera, []).&lt;&gt;outputs(camera, ['O', 'K']).&lt;&gt;input_types(camera, []).&lt;&gt;output_types(camera, [rgb, intrinsics]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== camera ===========&lt;&gt;section(camera, 'I/O').&lt;&gt;subsection(camera, 'imaging').&lt;&gt;description(camera, 'O is frames out of camera, K is camera intrinsics').&lt;&gt;visual_style(camera,  visual_style6).&lt;&gt;inputs(camera, []).&lt;&gt;outputs(camera, ['O', 'K']).&lt;&gt;input_types(camera, []).&lt;&gt;output_types(camera, [rgb, intrinsics]).&lt;&gt;image_name(camera, '/img/blocks/blocksheet1_06.png').&lt;&gt;prototype_coordinates(camera, 21, 5).&lt;&gt;</v>
       </c>
     </row>
     <row r="24" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4202,7 +4306,7 @@
       </c>
       <c r="AH24" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== eyes ===========&lt;&gt;section(eyes, 'I/O').&lt;&gt;subsection(eyes, 'imaging').&lt;&gt;description(eyes, 'input is commanded eye position, output is left and right eye cams').&lt;&gt;visual_style(eyes,  normal).&lt;&gt;inputs(eyes, [required('x'), required('y')]).&lt;&gt;outputs(eyes, ['OL', 'OR']).&lt;&gt;input_types(eyes, [proportion, proportion]).&lt;&gt;output_types(eyes, [rgb, rgb]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== eyes ===========&lt;&gt;section(eyes, 'I/O').&lt;&gt;subsection(eyes, 'imaging').&lt;&gt;description(eyes, 'input is commanded eye position, output is left and right eye cams').&lt;&gt;visual_style(eyes,  normal).&lt;&gt;inputs(eyes, [required('x'), required('y')]).&lt;&gt;outputs(eyes, ['OL', 'OR']).&lt;&gt;input_types(eyes, [proportion, proportion]).&lt;&gt;output_types(eyes, [rgb, rgb]).&lt;&gt;image_name(eyes, '/img/blocks/blocksheet1_07.png').&lt;&gt;</v>
       </c>
       <c r="AI24" t="str">
         <f t="shared" si="15"/>
@@ -4243,9 +4347,18 @@
       <c r="AS24">
         <v>1</v>
       </c>
+      <c r="BB24" t="s">
+        <v>278</v>
+      </c>
+      <c r="BC24">
+        <v>21</v>
+      </c>
+      <c r="BD24">
+        <v>6</v>
+      </c>
       <c r="BE24" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== eyes ===========&lt;&gt;section(eyes, 'I/O').&lt;&gt;subsection(eyes, 'imaging').&lt;&gt;description(eyes, 'input is commanded eye position, output is left and right eye cams').&lt;&gt;visual_style(eyes,  normal).&lt;&gt;inputs(eyes, [required('x'), required('y')]).&lt;&gt;outputs(eyes, ['OL', 'OR']).&lt;&gt;input_types(eyes, [proportion, proportion]).&lt;&gt;output_types(eyes, [rgb, rgb]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== eyes ===========&lt;&gt;section(eyes, 'I/O').&lt;&gt;subsection(eyes, 'imaging').&lt;&gt;description(eyes, 'input is commanded eye position, output is left and right eye cams').&lt;&gt;visual_style(eyes,  normal).&lt;&gt;inputs(eyes, [required('x'), required('y')]).&lt;&gt;outputs(eyes, ['OL', 'OR']).&lt;&gt;input_types(eyes, [proportion, proportion]).&lt;&gt;output_types(eyes, [rgb, rgb]).&lt;&gt;image_name(eyes, '/img/blocks/blocksheet1_07.png').&lt;&gt;prototype_coordinates(eyes, 21, 6).&lt;&gt;</v>
       </c>
     </row>
     <row r="25" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4588,7 +4701,7 @@
       </c>
       <c r="AH27" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== spectrum ===========&lt;&gt;section(spectrum, 'I/O').&lt;&gt;subsection(spectrum, 'imaging').&lt;&gt;description(spectrum, 'dancing spectrum display').&lt;&gt;visual_style(spectrum,  visual_style9).&lt;&gt;inputs(spectrum, [required('A')]).&lt;&gt;outputs(spectrum, []).&lt;&gt;input_types(spectrum, [sample]).&lt;&gt;output_types(spectrum, []).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== spectrum ===========&lt;&gt;section(spectrum, 'I/O').&lt;&gt;subsection(spectrum, 'imaging').&lt;&gt;description(spectrum, 'dancing spectrum display').&lt;&gt;visual_style(spectrum,  visual_style9).&lt;&gt;inputs(spectrum, [required('A')]).&lt;&gt;outputs(spectrum, []).&lt;&gt;input_types(spectrum, [sample]).&lt;&gt;output_types(spectrum, []).&lt;&gt;image_name(spectrum, '/img/blocks/blocksheet1_09.png').&lt;&gt;</v>
       </c>
       <c r="AI27" t="str">
         <f t="shared" si="15"/>
@@ -4629,9 +4742,18 @@
       <c r="AS27">
         <v>1</v>
       </c>
+      <c r="BB27" t="s">
+        <v>279</v>
+      </c>
+      <c r="BC27">
+        <v>21</v>
+      </c>
+      <c r="BD27">
+        <v>7</v>
+      </c>
       <c r="BE27" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== spectrum ===========&lt;&gt;section(spectrum, 'I/O').&lt;&gt;subsection(spectrum, 'imaging').&lt;&gt;description(spectrum, 'dancing spectrum display').&lt;&gt;visual_style(spectrum,  visual_style9).&lt;&gt;inputs(spectrum, [required('A')]).&lt;&gt;outputs(spectrum, []).&lt;&gt;input_types(spectrum, [sample]).&lt;&gt;output_types(spectrum, []).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== spectrum ===========&lt;&gt;section(spectrum, 'I/O').&lt;&gt;subsection(spectrum, 'imaging').&lt;&gt;description(spectrum, 'dancing spectrum display').&lt;&gt;visual_style(spectrum,  visual_style9).&lt;&gt;inputs(spectrum, [required('A')]).&lt;&gt;outputs(spectrum, []).&lt;&gt;input_types(spectrum, [sample]).&lt;&gt;output_types(spectrum, []).&lt;&gt;image_name(spectrum, '/img/blocks/blocksheet1_09.png').&lt;&gt;prototype_coordinates(spectrum, 21, 7).&lt;&gt;</v>
       </c>
     </row>
     <row r="28" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4838,7 +4960,7 @@
       </c>
       <c r="AH29" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== viewer ===========&lt;&gt;section(viewer, 'I/O').&lt;&gt;subsection(viewer, 'imaging').&lt;&gt;description(viewer, 'displays image').&lt;&gt;visual_style(viewer,  visual_style11).&lt;&gt;inputs(viewer, [required('A')]).&lt;&gt;outputs(viewer, []).&lt;&gt;input_types(viewer, [image]).&lt;&gt;output_types(viewer, []).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== viewer ===========&lt;&gt;section(viewer, 'I/O').&lt;&gt;subsection(viewer, 'imaging').&lt;&gt;description(viewer, 'displays image').&lt;&gt;visual_style(viewer,  visual_style11).&lt;&gt;inputs(viewer, [required('A')]).&lt;&gt;outputs(viewer, []).&lt;&gt;input_types(viewer, [image]).&lt;&gt;output_types(viewer, []).&lt;&gt;image_name(viewer, '/img/blocks/blocksheet1_13.png').&lt;&gt;</v>
       </c>
       <c r="AI29" t="str">
         <f t="shared" si="15"/>
@@ -4879,9 +5001,18 @@
       <c r="AS29">
         <v>1</v>
       </c>
+      <c r="BB29" t="s">
+        <v>280</v>
+      </c>
+      <c r="BC29">
+        <v>21</v>
+      </c>
+      <c r="BD29">
+        <v>8</v>
+      </c>
       <c r="BE29" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== viewer ===========&lt;&gt;section(viewer, 'I/O').&lt;&gt;subsection(viewer, 'imaging').&lt;&gt;description(viewer, 'displays image').&lt;&gt;visual_style(viewer,  visual_style11).&lt;&gt;inputs(viewer, [required('A')]).&lt;&gt;outputs(viewer, []).&lt;&gt;input_types(viewer, [image]).&lt;&gt;output_types(viewer, []).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== viewer ===========&lt;&gt;section(viewer, 'I/O').&lt;&gt;subsection(viewer, 'imaging').&lt;&gt;description(viewer, 'displays image').&lt;&gt;visual_style(viewer,  visual_style11).&lt;&gt;inputs(viewer, [required('A')]).&lt;&gt;outputs(viewer, []).&lt;&gt;input_types(viewer, [image]).&lt;&gt;output_types(viewer, []).&lt;&gt;image_name(viewer, '/img/blocks/blocksheet1_13.png').&lt;&gt;prototype_coordinates(viewer, 21, 8).&lt;&gt;</v>
       </c>
     </row>
     <row r="30" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4963,7 +5094,7 @@
       </c>
       <c r="AH30" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== kernal ===========&lt;&gt;section(kernal, 'I/O').&lt;&gt;subsection(kernal, 'imaging').&lt;&gt;description(kernal, 'kernal UI for defining kernals').&lt;&gt;visual_style(kernal,  visual_style12).&lt;&gt;inputs(kernal, []).&lt;&gt;outputs(kernal, ['O']).&lt;&gt;input_types(kernal, []).&lt;&gt;output_types(kernal, [kernal]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== kernal ===========&lt;&gt;section(kernal, 'I/O').&lt;&gt;subsection(kernal, 'imaging').&lt;&gt;description(kernal, 'kernal UI for defining kernals').&lt;&gt;visual_style(kernal,  visual_style12).&lt;&gt;inputs(kernal, []).&lt;&gt;outputs(kernal, ['O']).&lt;&gt;input_types(kernal, []).&lt;&gt;output_types(kernal, [kernal]).&lt;&gt;image_name(kernal, '/img/blocks/blocksheet1_14.png').&lt;&gt;</v>
       </c>
       <c r="AI30" t="str">
         <f t="shared" si="15"/>
@@ -5004,9 +5135,18 @@
       <c r="AS30">
         <v>1</v>
       </c>
+      <c r="BB30" t="s">
+        <v>281</v>
+      </c>
+      <c r="BC30">
+        <v>21</v>
+      </c>
+      <c r="BD30">
+        <v>9</v>
+      </c>
       <c r="BE30" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== kernal ===========&lt;&gt;section(kernal, 'I/O').&lt;&gt;subsection(kernal, 'imaging').&lt;&gt;description(kernal, 'kernal UI for defining kernals').&lt;&gt;visual_style(kernal,  visual_style12).&lt;&gt;inputs(kernal, []).&lt;&gt;outputs(kernal, ['O']).&lt;&gt;input_types(kernal, []).&lt;&gt;output_types(kernal, [kernal]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== kernal ===========&lt;&gt;section(kernal, 'I/O').&lt;&gt;subsection(kernal, 'imaging').&lt;&gt;description(kernal, 'kernal UI for defining kernals').&lt;&gt;visual_style(kernal,  visual_style12).&lt;&gt;inputs(kernal, []).&lt;&gt;outputs(kernal, ['O']).&lt;&gt;input_types(kernal, []).&lt;&gt;output_types(kernal, [kernal]).&lt;&gt;image_name(kernal, '/img/blocks/blocksheet1_14.png').&lt;&gt;prototype_coordinates(kernal, 21, 9).&lt;&gt;</v>
       </c>
     </row>
     <row r="31" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5199,7 +5339,7 @@
       </c>
       <c r="AH32" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== bodymask ===========&lt;&gt;section(bodymask, 'I/O').&lt;&gt;subsection(bodymask, 'body').&lt;&gt;description(bodymask, 'output is a vector of booleans for joints').&lt;&gt;visual_style(bodymask,  visual_style13).&lt;&gt;inputs(bodymask, []).&lt;&gt;outputs(bodymask, ['O']).&lt;&gt;input_types(bodymask, []).&lt;&gt;output_types(bodymask, [mask]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== bodymask ===========&lt;&gt;section(bodymask, 'I/O').&lt;&gt;subsection(bodymask, 'body').&lt;&gt;description(bodymask, 'output is a vector of booleans for joints').&lt;&gt;visual_style(bodymask,  visual_style13).&lt;&gt;inputs(bodymask, []).&lt;&gt;outputs(bodymask, ['O']).&lt;&gt;input_types(bodymask, []).&lt;&gt;output_types(bodymask, [mask]).&lt;&gt;image_name(bodymask, '/img/blocks/blocksheet1_10.png').&lt;&gt;</v>
       </c>
       <c r="AI32" t="str">
         <f t="shared" si="15"/>
@@ -5240,9 +5380,18 @@
       <c r="AS32">
         <v>1</v>
       </c>
+      <c r="BB32" t="s">
+        <v>282</v>
+      </c>
+      <c r="BC32">
+        <v>21</v>
+      </c>
+      <c r="BD32">
+        <v>10</v>
+      </c>
       <c r="BE32" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== bodymask ===========&lt;&gt;section(bodymask, 'I/O').&lt;&gt;subsection(bodymask, 'body').&lt;&gt;description(bodymask, 'output is a vector of booleans for joints').&lt;&gt;visual_style(bodymask,  visual_style13).&lt;&gt;inputs(bodymask, []).&lt;&gt;outputs(bodymask, ['O']).&lt;&gt;input_types(bodymask, []).&lt;&gt;output_types(bodymask, [mask]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== bodymask ===========&lt;&gt;section(bodymask, 'I/O').&lt;&gt;subsection(bodymask, 'body').&lt;&gt;description(bodymask, 'output is a vector of booleans for joints').&lt;&gt;visual_style(bodymask,  visual_style13).&lt;&gt;inputs(bodymask, []).&lt;&gt;outputs(bodymask, ['O']).&lt;&gt;input_types(bodymask, []).&lt;&gt;output_types(bodymask, [mask]).&lt;&gt;image_name(bodymask, '/img/blocks/blocksheet1_10.png').&lt;&gt;prototype_coordinates(bodymask, 21, 10).&lt;&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5321,7 +5470,7 @@
       </c>
       <c r="AH33" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== bodyposition ===========&lt;&gt;section(bodyposition, 'I/O').&lt;&gt;subsection(bodyposition, 'body').&lt;&gt;description(bodyposition, 'output is a vector of joint positions from physivcal bot').&lt;&gt;visual_style(bodyposition,  normal).&lt;&gt;inputs(bodyposition, []).&lt;&gt;outputs(bodyposition, ['O']).&lt;&gt;input_types(bodyposition, []).&lt;&gt;output_types(bodyposition, [joints]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== bodyposition ===========&lt;&gt;section(bodyposition, 'I/O').&lt;&gt;subsection(bodyposition, 'body').&lt;&gt;description(bodyposition, 'output is a vector of joint positions from physivcal bot').&lt;&gt;visual_style(bodyposition,  normal).&lt;&gt;inputs(bodyposition, []).&lt;&gt;outputs(bodyposition, ['O']).&lt;&gt;input_types(bodyposition, []).&lt;&gt;output_types(bodyposition, [joints]).&lt;&gt;image_name(bodyposition, '/img/blocks/blocksheet1_11.png').&lt;&gt;</v>
       </c>
       <c r="AI33" t="str">
         <f t="shared" si="15"/>
@@ -5362,9 +5511,18 @@
       <c r="AS33">
         <v>1</v>
       </c>
+      <c r="BB33" t="s">
+        <v>284</v>
+      </c>
+      <c r="BC33">
+        <v>21</v>
+      </c>
+      <c r="BD33">
+        <v>11</v>
+      </c>
       <c r="BE33" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== bodyposition ===========&lt;&gt;section(bodyposition, 'I/O').&lt;&gt;subsection(bodyposition, 'body').&lt;&gt;description(bodyposition, 'output is a vector of joint positions from physivcal bot').&lt;&gt;visual_style(bodyposition,  normal).&lt;&gt;inputs(bodyposition, []).&lt;&gt;outputs(bodyposition, ['O']).&lt;&gt;input_types(bodyposition, []).&lt;&gt;output_types(bodyposition, [joints]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== bodyposition ===========&lt;&gt;section(bodyposition, 'I/O').&lt;&gt;subsection(bodyposition, 'body').&lt;&gt;description(bodyposition, 'output is a vector of joint positions from physivcal bot').&lt;&gt;visual_style(bodyposition,  normal).&lt;&gt;inputs(bodyposition, []).&lt;&gt;outputs(bodyposition, ['O']).&lt;&gt;input_types(bodyposition, []).&lt;&gt;output_types(bodyposition, [joints]).&lt;&gt;image_name(bodyposition, '/img/blocks/blocksheet1_11.png').&lt;&gt;prototype_coordinates(bodyposition, 21, 11).&lt;&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5443,7 +5601,7 @@
       </c>
       <c r="AH34" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== bodypossim ===========&lt;&gt;section(bodypossim, 'I/O').&lt;&gt;subsection(bodypossim, 'body').&lt;&gt;description(bodypossim, 'as per bodyposition but from the simulator').&lt;&gt;visual_style(bodypossim,  normal).&lt;&gt;inputs(bodypossim, []).&lt;&gt;outputs(bodypossim, ['O']).&lt;&gt;input_types(bodypossim, []).&lt;&gt;output_types(bodypossim, [joints]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== bodypossim ===========&lt;&gt;section(bodypossim, 'I/O').&lt;&gt;subsection(bodypossim, 'body').&lt;&gt;description(bodypossim, 'as per bodyposition but from the simulator').&lt;&gt;visual_style(bodypossim,  normal).&lt;&gt;inputs(bodypossim, []).&lt;&gt;outputs(bodypossim, ['O']).&lt;&gt;input_types(bodypossim, []).&lt;&gt;output_types(bodypossim, [joints]).&lt;&gt;image_name(bodypossim, '/img/blocks/blocksheet1_16.png').&lt;&gt;</v>
       </c>
       <c r="AI34" t="str">
         <f t="shared" si="15"/>
@@ -5484,9 +5642,18 @@
       <c r="AS34">
         <v>1</v>
       </c>
+      <c r="BB34" t="s">
+        <v>285</v>
+      </c>
+      <c r="BC34">
+        <v>21</v>
+      </c>
+      <c r="BD34">
+        <v>12</v>
+      </c>
       <c r="BE34" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== bodypossim ===========&lt;&gt;section(bodypossim, 'I/O').&lt;&gt;subsection(bodypossim, 'body').&lt;&gt;description(bodypossim, 'as per bodyposition but from the simulator').&lt;&gt;visual_style(bodypossim,  normal).&lt;&gt;inputs(bodypossim, []).&lt;&gt;outputs(bodypossim, ['O']).&lt;&gt;input_types(bodypossim, []).&lt;&gt;output_types(bodypossim, [joints]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== bodypossim ===========&lt;&gt;section(bodypossim, 'I/O').&lt;&gt;subsection(bodypossim, 'body').&lt;&gt;description(bodypossim, 'as per bodyposition but from the simulator').&lt;&gt;visual_style(bodypossim,  normal).&lt;&gt;inputs(bodypossim, []).&lt;&gt;outputs(bodypossim, ['O']).&lt;&gt;input_types(bodypossim, []).&lt;&gt;output_types(bodypossim, [joints]).&lt;&gt;image_name(bodypossim, '/img/blocks/blocksheet1_16.png').&lt;&gt;prototype_coordinates(bodypossim, 21, 12).&lt;&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5570,7 +5737,7 @@
       </c>
       <c r="AH35" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== motors ===========&lt;&gt;section(motors, 'I/O').&lt;&gt;subsection(motors, 'body').&lt;&gt;description(motors, 'Send channels of vector A matching Mask to robot servos').&lt;&gt;visual_style(motors,  normal).&lt;&gt;inputs(motors, [required('A'), required('Mask')]).&lt;&gt;outputs(motors, []).&lt;&gt;input_types(motors, [joints, jointmask]).&lt;&gt;output_types(motors, []).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== motors ===========&lt;&gt;section(motors, 'I/O').&lt;&gt;subsection(motors, 'body').&lt;&gt;description(motors, 'Send channels of vector A matching Mask to robot servos').&lt;&gt;visual_style(motors,  normal).&lt;&gt;inputs(motors, [required('A'), required('Mask')]).&lt;&gt;outputs(motors, []).&lt;&gt;input_types(motors, [joints, jointmask]).&lt;&gt;output_types(motors, []).&lt;&gt;image_name(motors, '/img/blocks/blocksheet1_15.png').&lt;&gt;</v>
       </c>
       <c r="AI35" t="str">
         <f t="shared" si="15"/>
@@ -5611,9 +5778,18 @@
       <c r="AS35">
         <v>1</v>
       </c>
+      <c r="BB35" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC35">
+        <v>21</v>
+      </c>
+      <c r="BD35">
+        <v>13</v>
+      </c>
       <c r="BE35" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== motors ===========&lt;&gt;section(motors, 'I/O').&lt;&gt;subsection(motors, 'body').&lt;&gt;description(motors, 'Send channels of vector A matching Mask to robot servos').&lt;&gt;visual_style(motors,  normal).&lt;&gt;inputs(motors, [required('A'), required('Mask')]).&lt;&gt;outputs(motors, []).&lt;&gt;input_types(motors, [joints, jointmask]).&lt;&gt;output_types(motors, []).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== motors ===========&lt;&gt;section(motors, 'I/O').&lt;&gt;subsection(motors, 'body').&lt;&gt;description(motors, 'Send channels of vector A matching Mask to robot servos').&lt;&gt;visual_style(motors,  normal).&lt;&gt;inputs(motors, [required('A'), required('Mask')]).&lt;&gt;outputs(motors, []).&lt;&gt;input_types(motors, [joints, jointmask]).&lt;&gt;output_types(motors, []).&lt;&gt;image_name(motors, '/img/blocks/blocksheet1_15.png').&lt;&gt;prototype_coordinates(motors, 21, 13).&lt;&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5697,7 +5873,7 @@
       </c>
       <c r="AH36" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== motorsim ===========&lt;&gt;section(motorsim, 'I/O').&lt;&gt;subsection(motorsim, 'body').&lt;&gt;description(motorsim, 'As per motors, but to simulator').&lt;&gt;visual_style(motorsim,  normal).&lt;&gt;inputs(motorsim, [required('A'), required('Mask')]).&lt;&gt;outputs(motorsim, []).&lt;&gt;input_types(motorsim, [joints, jointmask]).&lt;&gt;output_types(motorsim, []).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== motorsim ===========&lt;&gt;section(motorsim, 'I/O').&lt;&gt;subsection(motorsim, 'body').&lt;&gt;description(motorsim, 'As per motors, but to simulator').&lt;&gt;visual_style(motorsim,  normal).&lt;&gt;inputs(motorsim, [required('A'), required('Mask')]).&lt;&gt;outputs(motorsim, []).&lt;&gt;input_types(motorsim, [joints, jointmask]).&lt;&gt;output_types(motorsim, []).&lt;&gt;image_name(motorsim, '/img/blocks/blocksheet1_17.png').&lt;&gt;</v>
       </c>
       <c r="AI36" t="str">
         <f t="shared" si="15"/>
@@ -5738,9 +5914,18 @@
       <c r="AS36">
         <v>1</v>
       </c>
+      <c r="BB36" t="s">
+        <v>286</v>
+      </c>
+      <c r="BC36">
+        <v>21</v>
+      </c>
+      <c r="BD36">
+        <v>14</v>
+      </c>
       <c r="BE36" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== motorsim ===========&lt;&gt;section(motorsim, 'I/O').&lt;&gt;subsection(motorsim, 'body').&lt;&gt;description(motorsim, 'As per motors, but to simulator').&lt;&gt;visual_style(motorsim,  normal).&lt;&gt;inputs(motorsim, [required('A'), required('Mask')]).&lt;&gt;outputs(motorsim, []).&lt;&gt;input_types(motorsim, [joints, jointmask]).&lt;&gt;output_types(motorsim, []).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== motorsim ===========&lt;&gt;section(motorsim, 'I/O').&lt;&gt;subsection(motorsim, 'body').&lt;&gt;description(motorsim, 'As per motors, but to simulator').&lt;&gt;visual_style(motorsim,  normal).&lt;&gt;inputs(motorsim, [required('A'), required('Mask')]).&lt;&gt;outputs(motorsim, []).&lt;&gt;input_types(motorsim, [joints, jointmask]).&lt;&gt;output_types(motorsim, []).&lt;&gt;image_name(motorsim, '/img/blocks/blocksheet1_17.png').&lt;&gt;prototype_coordinates(motorsim, 21, 14).&lt;&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7182,7 +7367,7 @@
       </c>
       <c r="AH46" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== vertpipe ===========&lt;&gt;section(vertpipe, 'connector').&lt;&gt;subsection(vertpipe, 'pipe').&lt;&gt;description(vertpipe, 'bidi pipe connection').&lt;&gt;visual_style(vertpipe,  visual_style21).&lt;&gt;inputs(vertpipe, [required('A')]).&lt;&gt;outputs(vertpipe, ['OA']).&lt;&gt;input_types(vertpipe, [any]).&lt;&gt;output_types(vertpipe, [any]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== vertpipe ===========&lt;&gt;section(vertpipe, 'connector').&lt;&gt;subsection(vertpipe, 'pipe').&lt;&gt;description(vertpipe, 'bidi pipe connection').&lt;&gt;visual_style(vertpipe,  visual_style21).&lt;&gt;inputs(vertpipe, [required('A')]).&lt;&gt;outputs(vertpipe, ['OA']).&lt;&gt;input_types(vertpipe, [any]).&lt;&gt;output_types(vertpipe, [any]).&lt;&gt;image_name(vertpipe, '/img/blocks/blocksheet0-_08.png').&lt;&gt;</v>
       </c>
       <c r="AI46" t="str">
         <f t="shared" si="42"/>
@@ -7220,9 +7405,18 @@
         <f t="shared" si="50"/>
         <v>[any]</v>
       </c>
+      <c r="BB46" t="s">
+        <v>287</v>
+      </c>
+      <c r="BC46">
+        <v>20</v>
+      </c>
+      <c r="BD46">
+        <v>7</v>
+      </c>
       <c r="BE46" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== vertpipe ===========&lt;&gt;section(vertpipe, 'connector').&lt;&gt;subsection(vertpipe, 'pipe').&lt;&gt;description(vertpipe, 'bidi pipe connection').&lt;&gt;visual_style(vertpipe,  visual_style21).&lt;&gt;inputs(vertpipe, [required('A')]).&lt;&gt;outputs(vertpipe, ['OA']).&lt;&gt;input_types(vertpipe, [any]).&lt;&gt;output_types(vertpipe, [any]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== vertpipe ===========&lt;&gt;section(vertpipe, 'connector').&lt;&gt;subsection(vertpipe, 'pipe').&lt;&gt;description(vertpipe, 'bidi pipe connection').&lt;&gt;visual_style(vertpipe,  visual_style21).&lt;&gt;inputs(vertpipe, [required('A')]).&lt;&gt;outputs(vertpipe, ['OA']).&lt;&gt;input_types(vertpipe, [any]).&lt;&gt;output_types(vertpipe, [any]).&lt;&gt;image_name(vertpipe, '/img/blocks/blocksheet0-_08.png').&lt;&gt;prototype_coordinates(vertpipe, 20, 7).&lt;&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
bug fix, outputs no longer listed as inputs
</commit_message>
<xml_diff>
--- a/doc/flo/Blocks.xlsx
+++ b/doc/flo/Blocks.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="555" windowWidth="12135" windowHeight="7770"/>
+    <workbookView xWindow="270" yWindow="555" windowWidth="12135" windowHeight="7770" tabRatio="842"/>
   </bookViews>
   <sheets>
     <sheet name="BlockTypes" sheetId="1" r:id="rId1"/>
     <sheet name="BaseTypes" sheetId="2" r:id="rId2"/>
     <sheet name="UI" sheetId="3" r:id="rId3"/>
+    <sheet name="BlockTypesHuman" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="296">
   <si>
     <t>Block Types</t>
   </si>
@@ -880,6 +881,30 @@
   </si>
   <si>
     <t>blocksheet0-_08.png</t>
+  </si>
+  <si>
+    <t>blocksheet0-_21.png</t>
+  </si>
+  <si>
+    <t>blocksheet0-_33.png</t>
+  </si>
+  <si>
+    <t>blocksheet0-_18.png</t>
+  </si>
+  <si>
+    <t>blocksheet0-_15.png</t>
+  </si>
+  <si>
+    <t>blocksheet0-_29.png</t>
+  </si>
+  <si>
+    <t>blocksheet0-_32.png</t>
+  </si>
+  <si>
+    <t>blocksheet0-_31.png</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -924,7 +949,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -981,11 +1006,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1028,10 +1073,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1342,7 +1417,7 @@
       <selection activeCell="AH1" sqref="AH1"/>
       <selection pane="topRight" activeCell="BE1" sqref="BE1"/>
       <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
-      <selection pane="bottomRight" activeCell="BD6" sqref="BD6"/>
+      <selection pane="bottomRight" activeCell="BE2" sqref="BE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1383,28 +1458,28 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14" t="s">
+      <c r="F1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14" t="s">
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14" t="s">
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
       <c r="T1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1441,10 +1516,10 @@
       <c r="BB1" t="s">
         <v>262</v>
       </c>
-      <c r="BC1" s="15" t="s">
+      <c r="BC1" s="24" t="s">
         <v>271</v>
       </c>
-      <c r="BD1" s="15"/>
+      <c r="BD1" s="24"/>
       <c r="BE1" t="s">
         <v>164</v>
       </c>
@@ -1558,7 +1633,7 @@
       </c>
       <c r="AH3" t="str">
         <f>IF(ISBLANK(E3),"","&lt;&gt;%  ===== "&amp;E3&amp;" ===========&lt;&gt;"&amp;AE3&amp;").&lt;&gt;inputs("&amp;E3&amp;", "&amp;Z3&amp;").&lt;&gt;outputs("&amp;E3&amp;", "&amp;AD3&amp;").&lt;&gt;input_types("&amp;E3&amp;", "&amp;AP3&amp;").&lt;&gt;output_types("&amp;E3&amp;", "&amp;AQ3&amp;").&lt;&gt;"&amp;IF(OR(ISBLANK(E3),ISBLANK(BB3)),"","image_name("&amp;E3&amp;", '/img/blocks/"&amp;BB3&amp;"').&lt;&gt;"))</f>
-        <v>&lt;&gt;%  ===== if ===========&lt;&gt;section(if, 'Control').&lt;&gt;subsection(if, 'Control').&lt;&gt;description(if, 'If Cond is true, O is A, else O is B').&lt;&gt;visual_style(if,  normal).&lt;&gt;inputs(if, [required('Cond'), required('A'), required('B')]).&lt;&gt;outputs(if, ['O']).&lt;&gt;input_types(if, [scalar, object, object]).&lt;&gt;output_types(if, [object]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== if ===========&lt;&gt;section(if, 'Control').&lt;&gt;subsection(if, 'Control').&lt;&gt;description(if, 'If Cond is true, O is A, else O is B').&lt;&gt;visual_style(if,  normal).&lt;&gt;inputs(if, [required('Cond'), required('A'), required('B')]).&lt;&gt;outputs(if, ['O']).&lt;&gt;input_types(if, [scalar, object, object]).&lt;&gt;output_types(if, [object]).&lt;&gt;image_name(if, '/img/blocks/blocksheet0-_21.png').&lt;&gt;</v>
       </c>
       <c r="AI3" t="str">
         <f>IF(ISBLANK(J3),"[","["&amp;J3)</f>
@@ -1614,9 +1689,18 @@
       <c r="BA3">
         <v>1</v>
       </c>
+      <c r="BB3" t="s">
+        <v>288</v>
+      </c>
+      <c r="BC3">
+        <v>22</v>
+      </c>
+      <c r="BD3">
+        <v>0</v>
+      </c>
       <c r="BE3" t="str">
-        <f>AH3&amp;IF(OR(ISBLANK(E3),ISBLANK(BC3)), "", "prototype_coordinates("&amp;E3&amp;", "&amp;BC3&amp;", "&amp;BD3&amp;").&lt;&gt;")</f>
-        <v>&lt;&gt;%  ===== if ===========&lt;&gt;section(if, 'Control').&lt;&gt;subsection(if, 'Control').&lt;&gt;description(if, 'If Cond is true, O is A, else O is B').&lt;&gt;visual_style(if,  normal).&lt;&gt;inputs(if, [required('Cond'), required('A'), required('B')]).&lt;&gt;outputs(if, ['O']).&lt;&gt;input_types(if, [scalar, object, object]).&lt;&gt;output_types(if, [object]).&lt;&gt;</v>
+        <f>AH3&amp;IF(OR(ISBLANK(E3),ISBLANK(BC3)), "", "prototype_coordinates("&amp;E3&amp;", "&amp;BC3&amp;", "&amp;BD3&amp;").&lt;&gt;icon_size("&amp;E3&amp;", "&amp;AZ3&amp;", "&amp;BA3&amp;").&lt;&gt;")</f>
+        <v>&lt;&gt;%  ===== if ===========&lt;&gt;section(if, 'Control').&lt;&gt;subsection(if, 'Control').&lt;&gt;description(if, 'If Cond is true, O is A, else O is B').&lt;&gt;visual_style(if,  normal).&lt;&gt;inputs(if, [required('Cond'), required('A'), required('B')]).&lt;&gt;outputs(if, ['O']).&lt;&gt;input_types(if, [scalar, object, object]).&lt;&gt;output_types(if, [object]).&lt;&gt;image_name(if, '/img/blocks/blocksheet0-_21.png').&lt;&gt;prototype_coordinates(if, 22, 0).&lt;&gt;icon_size(if, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1710,7 +1794,7 @@
       </c>
       <c r="AH4" t="str">
         <f t="shared" ref="AH4:AH67" si="14">IF(ISBLANK(E4),"","&lt;&gt;%  ===== "&amp;E4&amp;" ===========&lt;&gt;"&amp;AE4&amp;").&lt;&gt;inputs("&amp;E4&amp;", "&amp;Z4&amp;").&lt;&gt;outputs("&amp;E4&amp;", "&amp;AD4&amp;").&lt;&gt;input_types("&amp;E4&amp;", "&amp;AP4&amp;").&lt;&gt;output_types("&amp;E4&amp;", "&amp;AQ4&amp;").&lt;&gt;"&amp;IF(OR(ISBLANK(E4),ISBLANK(BB4)),"","image_name("&amp;E4&amp;", '/img/blocks/"&amp;BB4&amp;"').&lt;&gt;"))</f>
-        <v>&lt;&gt;%  ===== ifvar ===========&lt;&gt;section(ifvar, 'Control').&lt;&gt;subsection(ifvar, 'Control').&lt;&gt;description(ifvar, 'If the value of Va is true, O is A, else O is B. Var is some compile time variable (eg. DEV for development version).').&lt;&gt;visual_style(ifvar,  normal).&lt;&gt;inputs(ifvar, [required('Cond'), required('A'), required('B')]).&lt;&gt;outputs(ifvar, ['O']).&lt;&gt;input_types(ifvar, [string, object, object]).&lt;&gt;output_types(ifvar, [object]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== ifvar ===========&lt;&gt;section(ifvar, 'Control').&lt;&gt;subsection(ifvar, 'Control').&lt;&gt;description(ifvar, 'If the value of Va is true, O is A, else O is B. Var is some compile time variable (eg. DEV for development version).').&lt;&gt;visual_style(ifvar,  normal).&lt;&gt;inputs(ifvar, [required('Cond'), required('A'), required('B')]).&lt;&gt;outputs(ifvar, ['O']).&lt;&gt;input_types(ifvar, [string, object, object]).&lt;&gt;output_types(ifvar, [object]).&lt;&gt;image_name(ifvar, '/img/blocks/blocksheet0-_33.png').&lt;&gt;</v>
       </c>
       <c r="AI4" t="str">
         <f t="shared" ref="AI4:AI63" si="15">IF(ISBLANK(J4),"[","["&amp;J4)</f>
@@ -1766,9 +1850,18 @@
       <c r="BA4">
         <v>1</v>
       </c>
+      <c r="BB4" t="s">
+        <v>289</v>
+      </c>
+      <c r="BC4">
+        <v>22</v>
+      </c>
+      <c r="BD4">
+        <v>1</v>
+      </c>
       <c r="BE4" t="str">
-        <f t="shared" ref="BE4:BE67" si="24">AH4&amp;IF(OR(ISBLANK(E4),ISBLANK(BC4)), "", "prototype_coordinates("&amp;E4&amp;", "&amp;BC4&amp;", "&amp;BD4&amp;").&lt;&gt;")</f>
-        <v>&lt;&gt;%  ===== ifvar ===========&lt;&gt;section(ifvar, 'Control').&lt;&gt;subsection(ifvar, 'Control').&lt;&gt;description(ifvar, 'If the value of Va is true, O is A, else O is B. Var is some compile time variable (eg. DEV for development version).').&lt;&gt;visual_style(ifvar,  normal).&lt;&gt;inputs(ifvar, [required('Cond'), required('A'), required('B')]).&lt;&gt;outputs(ifvar, ['O']).&lt;&gt;input_types(ifvar, [string, object, object]).&lt;&gt;output_types(ifvar, [object]).&lt;&gt;</v>
+        <f t="shared" ref="BE4:BE67" si="24">AH4&amp;IF(OR(ISBLANK(E4),ISBLANK(BC4)), "", "prototype_coordinates("&amp;E4&amp;", "&amp;BC4&amp;", "&amp;BD4&amp;").&lt;&gt;icon_size("&amp;E4&amp;", "&amp;AZ4&amp;", "&amp;BA4&amp;").&lt;&gt;")</f>
+        <v>&lt;&gt;%  ===== ifvar ===========&lt;&gt;section(ifvar, 'Control').&lt;&gt;subsection(ifvar, 'Control').&lt;&gt;description(ifvar, 'If the value of Va is true, O is A, else O is B. Var is some compile time variable (eg. DEV for development version).').&lt;&gt;visual_style(ifvar,  normal).&lt;&gt;inputs(ifvar, [required('Cond'), required('A'), required('B')]).&lt;&gt;outputs(ifvar, ['O']).&lt;&gt;input_types(ifvar, [string, object, object]).&lt;&gt;output_types(ifvar, [object]).&lt;&gt;image_name(ifvar, '/img/blocks/blocksheet0-_33.png').&lt;&gt;prototype_coordinates(ifvar, 22, 1).&lt;&gt;icon_size(ifvar, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1856,7 +1949,7 @@
         <v>0</v>
       </c>
       <c r="AH5" t="str">
-        <f>IF(ISBLANK(E5),"","&lt;&gt;%  ===== "&amp;E5&amp;" ===========&lt;&gt;"&amp;AE5&amp;").&lt;&gt;inputs("&amp;E5&amp;", "&amp;Z5&amp;").&lt;&gt;outputs("&amp;E5&amp;", "&amp;AD5&amp;").&lt;&gt;input_types("&amp;E5&amp;", "&amp;AP5&amp;").&lt;&gt;output_types("&amp;E5&amp;", "&amp;AQ5&amp;").&lt;&gt;"&amp;IF(OR(ISBLANK(E5),ISBLANK(BB16)),"","image_name("&amp;E5&amp;", '/img/blocks/"&amp;BB16&amp;"').&lt;&gt;"))</f>
+        <f t="shared" si="14"/>
         <v>&lt;&gt;%  ===== flipflop ===========&lt;&gt;section(flipflop, 'Control').&lt;&gt;subsection(flipflop, 'Control').&lt;&gt;description(flipflop, 'a jk flipflop').&lt;&gt;visual_style(flipflop,  normal).&lt;&gt;inputs(flipflop, [required('J'), required('K')]).&lt;&gt;outputs(flipflop, ['O']).&lt;&gt;input_types(flipflop, [pulse, pulse]).&lt;&gt;output_types(flipflop, [int]).&lt;&gt;image_name(flipflop, '/img/blocks/blocksheet1_01.png').&lt;&gt;</v>
       </c>
       <c r="AI5" t="str">
@@ -1898,9 +1991,18 @@
       <c r="AS5">
         <v>1</v>
       </c>
+      <c r="BB5" t="s">
+        <v>272</v>
+      </c>
+      <c r="BC5">
+        <v>22</v>
+      </c>
+      <c r="BD5">
+        <v>2</v>
+      </c>
       <c r="BE5" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== flipflop ===========&lt;&gt;section(flipflop, 'Control').&lt;&gt;subsection(flipflop, 'Control').&lt;&gt;description(flipflop, 'a jk flipflop').&lt;&gt;visual_style(flipflop,  normal).&lt;&gt;inputs(flipflop, [required('J'), required('K')]).&lt;&gt;outputs(flipflop, ['O']).&lt;&gt;input_types(flipflop, [pulse, pulse]).&lt;&gt;output_types(flipflop, [int]).&lt;&gt;image_name(flipflop, '/img/blocks/blocksheet1_01.png').&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== flipflop ===========&lt;&gt;section(flipflop, 'Control').&lt;&gt;subsection(flipflop, 'Control').&lt;&gt;description(flipflop, 'a jk flipflop').&lt;&gt;visual_style(flipflop,  normal).&lt;&gt;inputs(flipflop, [required('J'), required('K')]).&lt;&gt;outputs(flipflop, ['O']).&lt;&gt;input_types(flipflop, [pulse, pulse]).&lt;&gt;output_types(flipflop, [int]).&lt;&gt;image_name(flipflop, '/img/blocks/blocksheet1_01.png').&lt;&gt;prototype_coordinates(flipflop, 22, 2).&lt;&gt;icon_size(flipflop, , ).&lt;&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2100,7 +2202,7 @@
       </c>
       <c r="AH7" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== isolate ===========&lt;&gt;section(isolate, 'Editor Support').&lt;&gt;subsection(isolate, 'Editor Support').&lt;&gt;description(isolate, 'if the connection to A is visible, runs the network beyond A and passes A to O. Otherwise passes default to O. Used during development to prevent, for example, having to run the entire sound system because the sound system sends a hint to the CV system.').&lt;&gt;visual_style(isolate,  normal).&lt;&gt;inputs(isolate, [required('A'), required('Default')]).&lt;&gt;outputs(isolate, ['O']).&lt;&gt;input_types(isolate, [object, object]).&lt;&gt;output_types(isolate, [object]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== isolate ===========&lt;&gt;section(isolate, 'Editor Support').&lt;&gt;subsection(isolate, 'Editor Support').&lt;&gt;description(isolate, 'if the connection to A is visible, runs the network beyond A and passes A to O. Otherwise passes default to O. Used during development to prevent, for example, having to run the entire sound system because the sound system sends a hint to the CV system.').&lt;&gt;visual_style(isolate,  normal).&lt;&gt;inputs(isolate, [required('A'), required('Default')]).&lt;&gt;outputs(isolate, ['O']).&lt;&gt;input_types(isolate, [object, object]).&lt;&gt;output_types(isolate, [object]).&lt;&gt;image_name(isolate, '/img/blocks/blocksheet0-_18.png').&lt;&gt;</v>
       </c>
       <c r="AI7" t="str">
         <f t="shared" si="15"/>
@@ -2156,9 +2258,18 @@
       <c r="BA7">
         <v>1</v>
       </c>
+      <c r="BB7" t="s">
+        <v>290</v>
+      </c>
+      <c r="BC7">
+        <v>22</v>
+      </c>
+      <c r="BD7">
+        <v>3</v>
+      </c>
       <c r="BE7" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== isolate ===========&lt;&gt;section(isolate, 'Editor Support').&lt;&gt;subsection(isolate, 'Editor Support').&lt;&gt;description(isolate, 'if the connection to A is visible, runs the network beyond A and passes A to O. Otherwise passes default to O. Used during development to prevent, for example, having to run the entire sound system because the sound system sends a hint to the CV system.').&lt;&gt;visual_style(isolate,  normal).&lt;&gt;inputs(isolate, [required('A'), required('Default')]).&lt;&gt;outputs(isolate, ['O']).&lt;&gt;input_types(isolate, [object, object]).&lt;&gt;output_types(isolate, [object]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== isolate ===========&lt;&gt;section(isolate, 'Editor Support').&lt;&gt;subsection(isolate, 'Editor Support').&lt;&gt;description(isolate, 'if the connection to A is visible, runs the network beyond A and passes A to O. Otherwise passes default to O. Used during development to prevent, for example, having to run the entire sound system because the sound system sends a hint to the CV system.').&lt;&gt;visual_style(isolate,  normal).&lt;&gt;inputs(isolate, [required('A'), required('Default')]).&lt;&gt;outputs(isolate, ['O']).&lt;&gt;input_types(isolate, [object, object]).&lt;&gt;output_types(isolate, [object]).&lt;&gt;image_name(isolate, '/img/blocks/blocksheet0-_18.png').&lt;&gt;prototype_coordinates(isolate, 22, 3).&lt;&gt;icon_size(isolate, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2240,7 +2351,7 @@
       </c>
       <c r="AH8" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== inputparam ===========&lt;&gt;section(inputparam, 'Editor Support').&lt;&gt;subsection(inputparam, 'Editor Support').&lt;&gt;description(inputparam, 'used when defining new blocks').&lt;&gt;visual_style(inputparam,  visual_style0).&lt;&gt;inputs(inputparam, []).&lt;&gt;outputs(inputparam, ['O']).&lt;&gt;input_types(inputparam, []).&lt;&gt;output_types(inputparam, [object]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== inputparam ===========&lt;&gt;section(inputparam, 'Editor Support').&lt;&gt;subsection(inputparam, 'Editor Support').&lt;&gt;description(inputparam, 'used when defining new blocks').&lt;&gt;visual_style(inputparam,  visual_style0).&lt;&gt;inputs(inputparam, []).&lt;&gt;outputs(inputparam, ['O']).&lt;&gt;input_types(inputparam, []).&lt;&gt;output_types(inputparam, [object]).&lt;&gt;image_name(inputparam, '/img/blocks/blocksheet0-_15.png').&lt;&gt;</v>
       </c>
       <c r="AI8" t="str">
         <f t="shared" si="15"/>
@@ -2296,9 +2407,18 @@
       <c r="BA8">
         <v>1</v>
       </c>
+      <c r="BB8" t="s">
+        <v>291</v>
+      </c>
+      <c r="BC8">
+        <v>22</v>
+      </c>
+      <c r="BD8">
+        <v>4</v>
+      </c>
       <c r="BE8" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== inputparam ===========&lt;&gt;section(inputparam, 'Editor Support').&lt;&gt;subsection(inputparam, 'Editor Support').&lt;&gt;description(inputparam, 'used when defining new blocks').&lt;&gt;visual_style(inputparam,  visual_style0).&lt;&gt;inputs(inputparam, []).&lt;&gt;outputs(inputparam, ['O']).&lt;&gt;input_types(inputparam, []).&lt;&gt;output_types(inputparam, [object]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== inputparam ===========&lt;&gt;section(inputparam, 'Editor Support').&lt;&gt;subsection(inputparam, 'Editor Support').&lt;&gt;description(inputparam, 'used when defining new blocks').&lt;&gt;visual_style(inputparam,  visual_style0).&lt;&gt;inputs(inputparam, []).&lt;&gt;outputs(inputparam, ['O']).&lt;&gt;input_types(inputparam, []).&lt;&gt;output_types(inputparam, [object]).&lt;&gt;image_name(inputparam, '/img/blocks/blocksheet0-_15.png').&lt;&gt;prototype_coordinates(inputparam, 22, 4).&lt;&gt;icon_size(inputparam, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2380,7 +2500,7 @@
       </c>
       <c r="AH9" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== outputparam ===========&lt;&gt;section(outputparam, 'Editor Support').&lt;&gt;subsection(outputparam, 'Editor Support').&lt;&gt;description(outputparam, 'used when defining new blocks').&lt;&gt;visual_style(outputparam,  visual_style1).&lt;&gt;inputs(outputparam, [required('A')]).&lt;&gt;outputs(outputparam, []).&lt;&gt;input_types(outputparam, [object]).&lt;&gt;output_types(outputparam, []).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== outputparam ===========&lt;&gt;section(outputparam, 'Editor Support').&lt;&gt;subsection(outputparam, 'Editor Support').&lt;&gt;description(outputparam, 'used when defining new blocks').&lt;&gt;visual_style(outputparam,  visual_style1).&lt;&gt;inputs(outputparam, [required('A')]).&lt;&gt;outputs(outputparam, []).&lt;&gt;input_types(outputparam, [object]).&lt;&gt;output_types(outputparam, []).&lt;&gt;image_name(outputparam, '/img/blocks/blocksheet0-_29.png').&lt;&gt;</v>
       </c>
       <c r="AI9" t="str">
         <f t="shared" si="15"/>
@@ -2436,9 +2556,18 @@
       <c r="BA9">
         <v>1</v>
       </c>
+      <c r="BB9" t="s">
+        <v>292</v>
+      </c>
+      <c r="BC9">
+        <v>22</v>
+      </c>
+      <c r="BD9">
+        <v>5</v>
+      </c>
       <c r="BE9" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== outputparam ===========&lt;&gt;section(outputparam, 'Editor Support').&lt;&gt;subsection(outputparam, 'Editor Support').&lt;&gt;description(outputparam, 'used when defining new blocks').&lt;&gt;visual_style(outputparam,  visual_style1).&lt;&gt;inputs(outputparam, [required('A')]).&lt;&gt;outputs(outputparam, []).&lt;&gt;input_types(outputparam, [object]).&lt;&gt;output_types(outputparam, []).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== outputparam ===========&lt;&gt;section(outputparam, 'Editor Support').&lt;&gt;subsection(outputparam, 'Editor Support').&lt;&gt;description(outputparam, 'used when defining new blocks').&lt;&gt;visual_style(outputparam,  visual_style1).&lt;&gt;inputs(outputparam, [required('A')]).&lt;&gt;outputs(outputparam, []).&lt;&gt;input_types(outputparam, [object]).&lt;&gt;output_types(outputparam, []).&lt;&gt;image_name(outputparam, '/img/blocks/blocksheet0-_29.png').&lt;&gt;prototype_coordinates(outputparam, 22, 5).&lt;&gt;icon_size(outputparam, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2647,7 +2776,7 @@
       </c>
       <c r="AH11" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== func ===========&lt;&gt;section(func, 'Math').&lt;&gt;subsection(func, 'Math').&lt;&gt;description(func, 'This special block has a textbox for a formula. So if you type 3x+2 you see an input parameter x. Operator meaning depends on whats connected to x (scalar or vector). Understands LSL angle bracket quat syntax').&lt;&gt;visual_style(func,  normal).&lt;&gt;inputs(func, [required('A'), required('B'), required('C')]).&lt;&gt;outputs(func, ['O']).&lt;&gt;input_types(func, [scalar, scalar, scalar, scalar]).&lt;&gt;output_types(func, [object]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== func ===========&lt;&gt;section(func, 'Math').&lt;&gt;subsection(func, 'Math').&lt;&gt;description(func, 'This special block has a textbox for a formula. So if you type 3x+2 you see an input parameter x. Operator meaning depends on whats connected to x (scalar or vector). Understands LSL angle bracket quat syntax').&lt;&gt;visual_style(func,  normal).&lt;&gt;inputs(func, [required('A'), required('B'), required('C')]).&lt;&gt;outputs(func, ['O']).&lt;&gt;input_types(func, [scalar, scalar, scalar, scalar]).&lt;&gt;output_types(func, [object]).&lt;&gt;image_name(func, '/img/blocks/blocksheet0-_32.png').&lt;&gt;</v>
       </c>
       <c r="AI11" t="str">
         <f t="shared" si="15"/>
@@ -2703,9 +2832,18 @@
       <c r="BA11">
         <v>1</v>
       </c>
+      <c r="BB11" t="s">
+        <v>293</v>
+      </c>
+      <c r="BC11">
+        <v>23</v>
+      </c>
+      <c r="BD11">
+        <v>0</v>
+      </c>
       <c r="BE11" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== func ===========&lt;&gt;section(func, 'Math').&lt;&gt;subsection(func, 'Math').&lt;&gt;description(func, 'This special block has a textbox for a formula. So if you type 3x+2 you see an input parameter x. Operator meaning depends on whats connected to x (scalar or vector). Understands LSL angle bracket quat syntax').&lt;&gt;visual_style(func,  normal).&lt;&gt;inputs(func, [required('A'), required('B'), required('C')]).&lt;&gt;outputs(func, ['O']).&lt;&gt;input_types(func, [scalar, scalar, scalar, scalar]).&lt;&gt;output_types(func, [object]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== func ===========&lt;&gt;section(func, 'Math').&lt;&gt;subsection(func, 'Math').&lt;&gt;description(func, 'This special block has a textbox for a formula. So if you type 3x+2 you see an input parameter x. Operator meaning depends on whats connected to x (scalar or vector). Understands LSL angle bracket quat syntax').&lt;&gt;visual_style(func,  normal).&lt;&gt;inputs(func, [required('A'), required('B'), required('C')]).&lt;&gt;outputs(func, ['O']).&lt;&gt;input_types(func, [scalar, scalar, scalar, scalar]).&lt;&gt;output_types(func, [object]).&lt;&gt;image_name(func, '/img/blocks/blocksheet0-_32.png').&lt;&gt;prototype_coordinates(func, 23, 0).&lt;&gt;icon_size(func, 2, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2900,7 +3038,7 @@
       </c>
       <c r="AH13" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== delay ===========&lt;&gt;section(delay, 'Misc').&lt;&gt;subsection(delay, 'Misc').&lt;&gt;description(delay, 'O is the previous stable value of A').&lt;&gt;visual_style(delay,  normal).&lt;&gt;inputs(delay, [required('A')]).&lt;&gt;outputs(delay, ['O']).&lt;&gt;input_types(delay, [object]).&lt;&gt;output_types(delay, [object]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== delay ===========&lt;&gt;section(delay, 'Misc').&lt;&gt;subsection(delay, 'Misc').&lt;&gt;description(delay, 'O is the previous stable value of A').&lt;&gt;visual_style(delay,  normal).&lt;&gt;inputs(delay, [required('A')]).&lt;&gt;outputs(delay, ['O']).&lt;&gt;input_types(delay, [object]).&lt;&gt;output_types(delay, [object]).&lt;&gt;image_name(delay, '/img/blocks/blocksheet0-_31.png').&lt;&gt;</v>
       </c>
       <c r="AI13" t="str">
         <f t="shared" si="15"/>
@@ -2956,9 +3094,18 @@
       <c r="BA13">
         <v>1</v>
       </c>
+      <c r="BB13" t="s">
+        <v>294</v>
+      </c>
+      <c r="BC13">
+        <v>23</v>
+      </c>
+      <c r="BD13">
+        <v>1</v>
+      </c>
       <c r="BE13" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== delay ===========&lt;&gt;section(delay, 'Misc').&lt;&gt;subsection(delay, 'Misc').&lt;&gt;description(delay, 'O is the previous stable value of A').&lt;&gt;visual_style(delay,  normal).&lt;&gt;inputs(delay, [required('A')]).&lt;&gt;outputs(delay, ['O']).&lt;&gt;input_types(delay, [object]).&lt;&gt;output_types(delay, [object]).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== delay ===========&lt;&gt;section(delay, 'Misc').&lt;&gt;subsection(delay, 'Misc').&lt;&gt;description(delay, 'O is the previous stable value of A').&lt;&gt;visual_style(delay,  normal).&lt;&gt;inputs(delay, [required('A')]).&lt;&gt;outputs(delay, ['O']).&lt;&gt;input_types(delay, [object]).&lt;&gt;output_types(delay, [object]).&lt;&gt;image_name(delay, '/img/blocks/blocksheet0-_31.png').&lt;&gt;prototype_coordinates(delay, 23, 1).&lt;&gt;icon_size(delay, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3303,6 +3450,12 @@
       <c r="AS16">
         <v>1</v>
       </c>
+      <c r="AZ16">
+        <v>1</v>
+      </c>
+      <c r="BA16">
+        <v>1</v>
+      </c>
       <c r="BB16" t="s">
         <v>272</v>
       </c>
@@ -3314,7 +3467,7 @@
       </c>
       <c r="BE16" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== pulse ===========&lt;&gt;section(pulse, 'I/O').&lt;&gt;subsection(pulse, 'scalar').&lt;&gt;description(pulse, 'Is 1 on the next frame after mouseup').&lt;&gt;visual_style(pulse,  visual_style2).&lt;&gt;inputs(pulse, []).&lt;&gt;outputs(pulse, ['O']).&lt;&gt;input_types(pulse, []).&lt;&gt;output_types(pulse, [pulse]).&lt;&gt;image_name(pulse, '/img/blocks/blocksheet1_01.png').&lt;&gt;prototype_coordinates(pulse, 21, 0).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== pulse ===========&lt;&gt;section(pulse, 'I/O').&lt;&gt;subsection(pulse, 'scalar').&lt;&gt;description(pulse, 'Is 1 on the next frame after mouseup').&lt;&gt;visual_style(pulse,  visual_style2).&lt;&gt;inputs(pulse, []).&lt;&gt;outputs(pulse, ['O']).&lt;&gt;input_types(pulse, []).&lt;&gt;output_types(pulse, [pulse]).&lt;&gt;image_name(pulse, '/img/blocks/blocksheet1_01.png').&lt;&gt;prototype_coordinates(pulse, 21, 0).&lt;&gt;icon_size(pulse, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="17" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3437,6 +3590,12 @@
       <c r="AS17">
         <v>1</v>
       </c>
+      <c r="AZ17">
+        <v>1</v>
+      </c>
+      <c r="BA17">
+        <v>1</v>
+      </c>
       <c r="BB17" t="s">
         <v>273</v>
       </c>
@@ -3449,7 +3608,7 @@
       </c>
       <c r="BE17" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== proportion ===========&lt;&gt;section(proportion, 'I/O').&lt;&gt;subsection(proportion, 'scalar').&lt;&gt;description(proportion, 'slider value from 0-1').&lt;&gt;visual_style(proportion,  visual_style3).&lt;&gt;inputs(proportion, []).&lt;&gt;outputs(proportion, ['O']).&lt;&gt;input_types(proportion, []).&lt;&gt;output_types(proportion, [proportion]).&lt;&gt;image_name(proportion, '/img/blocks/blocksheet1_02.png').&lt;&gt;prototype_coordinates(proportion, 21, 1).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== proportion ===========&lt;&gt;section(proportion, 'I/O').&lt;&gt;subsection(proportion, 'scalar').&lt;&gt;description(proportion, 'slider value from 0-1').&lt;&gt;visual_style(proportion,  visual_style3).&lt;&gt;inputs(proportion, []).&lt;&gt;outputs(proportion, ['O']).&lt;&gt;input_types(proportion, []).&lt;&gt;output_types(proportion, [proportion]).&lt;&gt;image_name(proportion, '/img/blocks/blocksheet1_02.png').&lt;&gt;prototype_coordinates(proportion, 21, 1).&lt;&gt;icon_size(proportion, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="18" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3572,6 +3731,12 @@
       <c r="AS18">
         <v>1</v>
       </c>
+      <c r="AZ18">
+        <v>1</v>
+      </c>
+      <c r="BA18">
+        <v>1</v>
+      </c>
       <c r="BB18" t="s">
         <v>274</v>
       </c>
@@ -3584,7 +3749,7 @@
       </c>
       <c r="BE18" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== floatval ===========&lt;&gt;section(floatval, 'I/O').&lt;&gt;subsection(floatval, 'scalar').&lt;&gt;description(floatval, 'float value that varies over -inf to +inf').&lt;&gt;visual_style(floatval,  visual_style4).&lt;&gt;inputs(floatval, []).&lt;&gt;outputs(floatval, ['O']).&lt;&gt;input_types(floatval, []).&lt;&gt;output_types(floatval, [float]).&lt;&gt;image_name(floatval, '/img/blocks/blocksheet1_03.png').&lt;&gt;prototype_coordinates(floatval, 21, 2).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== floatval ===========&lt;&gt;section(floatval, 'I/O').&lt;&gt;subsection(floatval, 'scalar').&lt;&gt;description(floatval, 'float value that varies over -inf to +inf').&lt;&gt;visual_style(floatval,  visual_style4).&lt;&gt;inputs(floatval, []).&lt;&gt;outputs(floatval, ['O']).&lt;&gt;input_types(floatval, []).&lt;&gt;output_types(floatval, [float]).&lt;&gt;image_name(floatval, '/img/blocks/blocksheet1_03.png').&lt;&gt;prototype_coordinates(floatval, 21, 2).&lt;&gt;icon_size(floatval, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="19" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3815,6 +3980,12 @@
       <c r="AS20">
         <v>1</v>
       </c>
+      <c r="AZ20">
+        <v>1</v>
+      </c>
+      <c r="BA20">
+        <v>1</v>
+      </c>
       <c r="BB20" t="s">
         <v>275</v>
       </c>
@@ -3826,7 +3997,7 @@
       </c>
       <c r="BE20" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== mic ===========&lt;&gt;section(mic, 'I/O').&lt;&gt;subsection(mic, 'sound').&lt;&gt;description(mic, 'samples from mic').&lt;&gt;visual_style(mic,  normal).&lt;&gt;inputs(mic, []).&lt;&gt;outputs(mic, ['O']).&lt;&gt;input_types(mic, []).&lt;&gt;output_types(mic, [sample]).&lt;&gt;image_name(mic, '/img/blocks/blocksheet1_04.png').&lt;&gt;prototype_coordinates(mic, 21, 3).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== mic ===========&lt;&gt;section(mic, 'I/O').&lt;&gt;subsection(mic, 'sound').&lt;&gt;description(mic, 'samples from mic').&lt;&gt;visual_style(mic,  normal).&lt;&gt;inputs(mic, []).&lt;&gt;outputs(mic, ['O']).&lt;&gt;input_types(mic, []).&lt;&gt;output_types(mic, [sample]).&lt;&gt;image_name(mic, '/img/blocks/blocksheet1_04.png').&lt;&gt;prototype_coordinates(mic, 21, 3).&lt;&gt;icon_size(mic, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="21" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3949,6 +4120,12 @@
       <c r="AS21">
         <v>1</v>
       </c>
+      <c r="AZ21">
+        <v>1</v>
+      </c>
+      <c r="BA21">
+        <v>1</v>
+      </c>
       <c r="BB21" t="s">
         <v>276</v>
       </c>
@@ -3960,7 +4137,7 @@
       </c>
       <c r="BE21" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== listen ===========&lt;&gt;section(listen, 'I/O').&lt;&gt;subsection(listen, 'sound').&lt;&gt;description(listen, 'Sends sound to default output').&lt;&gt;visual_style(listen,  visual_style5).&lt;&gt;inputs(listen, [required('A')]).&lt;&gt;outputs(listen, []).&lt;&gt;input_types(listen, [sample]).&lt;&gt;output_types(listen, []).&lt;&gt;image_name(listen, '/img/blocks/blocksheet1_05.png').&lt;&gt;prototype_coordinates(listen, 21, 4).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== listen ===========&lt;&gt;section(listen, 'I/O').&lt;&gt;subsection(listen, 'sound').&lt;&gt;description(listen, 'Sends sound to default output').&lt;&gt;visual_style(listen,  visual_style5).&lt;&gt;inputs(listen, [required('A')]).&lt;&gt;outputs(listen, []).&lt;&gt;input_types(listen, [sample]).&lt;&gt;output_types(listen, []).&lt;&gt;image_name(listen, '/img/blocks/blocksheet1_05.png').&lt;&gt;prototype_coordinates(listen, 21, 4).&lt;&gt;icon_size(listen, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="22" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4200,6 +4377,12 @@
       <c r="AS23">
         <v>1</v>
       </c>
+      <c r="AZ23">
+        <v>1</v>
+      </c>
+      <c r="BA23">
+        <v>1</v>
+      </c>
       <c r="BB23" t="s">
         <v>277</v>
       </c>
@@ -4211,7 +4394,7 @@
       </c>
       <c r="BE23" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== camera ===========&lt;&gt;section(camera, 'I/O').&lt;&gt;subsection(camera, 'imaging').&lt;&gt;description(camera, 'O is frames out of camera, K is camera intrinsics').&lt;&gt;visual_style(camera,  visual_style6).&lt;&gt;inputs(camera, []).&lt;&gt;outputs(camera, ['O', 'K']).&lt;&gt;input_types(camera, []).&lt;&gt;output_types(camera, [rgb, intrinsics]).&lt;&gt;image_name(camera, '/img/blocks/blocksheet1_06.png').&lt;&gt;prototype_coordinates(camera, 21, 5).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== camera ===========&lt;&gt;section(camera, 'I/O').&lt;&gt;subsection(camera, 'imaging').&lt;&gt;description(camera, 'O is frames out of camera, K is camera intrinsics').&lt;&gt;visual_style(camera,  visual_style6).&lt;&gt;inputs(camera, []).&lt;&gt;outputs(camera, ['O', 'K']).&lt;&gt;input_types(camera, []).&lt;&gt;output_types(camera, [rgb, intrinsics]).&lt;&gt;image_name(camera, '/img/blocks/blocksheet1_06.png').&lt;&gt;prototype_coordinates(camera, 21, 5).&lt;&gt;icon_size(camera, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="24" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4347,6 +4530,12 @@
       <c r="AS24">
         <v>1</v>
       </c>
+      <c r="AZ24">
+        <v>2</v>
+      </c>
+      <c r="BA24">
+        <v>1</v>
+      </c>
       <c r="BB24" t="s">
         <v>278</v>
       </c>
@@ -4358,7 +4547,7 @@
       </c>
       <c r="BE24" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== eyes ===========&lt;&gt;section(eyes, 'I/O').&lt;&gt;subsection(eyes, 'imaging').&lt;&gt;description(eyes, 'input is commanded eye position, output is left and right eye cams').&lt;&gt;visual_style(eyes,  normal).&lt;&gt;inputs(eyes, [required('x'), required('y')]).&lt;&gt;outputs(eyes, ['OL', 'OR']).&lt;&gt;input_types(eyes, [proportion, proportion]).&lt;&gt;output_types(eyes, [rgb, rgb]).&lt;&gt;image_name(eyes, '/img/blocks/blocksheet1_07.png').&lt;&gt;prototype_coordinates(eyes, 21, 6).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== eyes ===========&lt;&gt;section(eyes, 'I/O').&lt;&gt;subsection(eyes, 'imaging').&lt;&gt;description(eyes, 'input is commanded eye position, output is left and right eye cams').&lt;&gt;visual_style(eyes,  normal).&lt;&gt;inputs(eyes, [required('x'), required('y')]).&lt;&gt;outputs(eyes, ['OL', 'OR']).&lt;&gt;input_types(eyes, [proportion, proportion]).&lt;&gt;output_types(eyes, [rgb, rgb]).&lt;&gt;image_name(eyes, '/img/blocks/blocksheet1_07.png').&lt;&gt;prototype_coordinates(eyes, 21, 6).&lt;&gt;icon_size(eyes, 2, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="25" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4742,6 +4931,12 @@
       <c r="AS27">
         <v>1</v>
       </c>
+      <c r="AZ27">
+        <v>1</v>
+      </c>
+      <c r="BA27">
+        <v>1</v>
+      </c>
       <c r="BB27" t="s">
         <v>279</v>
       </c>
@@ -4753,7 +4948,7 @@
       </c>
       <c r="BE27" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== spectrum ===========&lt;&gt;section(spectrum, 'I/O').&lt;&gt;subsection(spectrum, 'imaging').&lt;&gt;description(spectrum, 'dancing spectrum display').&lt;&gt;visual_style(spectrum,  visual_style9).&lt;&gt;inputs(spectrum, [required('A')]).&lt;&gt;outputs(spectrum, []).&lt;&gt;input_types(spectrum, [sample]).&lt;&gt;output_types(spectrum, []).&lt;&gt;image_name(spectrum, '/img/blocks/blocksheet1_09.png').&lt;&gt;prototype_coordinates(spectrum, 21, 7).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== spectrum ===========&lt;&gt;section(spectrum, 'I/O').&lt;&gt;subsection(spectrum, 'imaging').&lt;&gt;description(spectrum, 'dancing spectrum display').&lt;&gt;visual_style(spectrum,  visual_style9).&lt;&gt;inputs(spectrum, [required('A')]).&lt;&gt;outputs(spectrum, []).&lt;&gt;input_types(spectrum, [sample]).&lt;&gt;output_types(spectrum, []).&lt;&gt;image_name(spectrum, '/img/blocks/blocksheet1_09.png').&lt;&gt;prototype_coordinates(spectrum, 21, 7).&lt;&gt;icon_size(spectrum, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="28" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5001,6 +5196,12 @@
       <c r="AS29">
         <v>1</v>
       </c>
+      <c r="AZ29">
+        <v>1</v>
+      </c>
+      <c r="BA29">
+        <v>1</v>
+      </c>
       <c r="BB29" t="s">
         <v>280</v>
       </c>
@@ -5012,7 +5213,7 @@
       </c>
       <c r="BE29" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== viewer ===========&lt;&gt;section(viewer, 'I/O').&lt;&gt;subsection(viewer, 'imaging').&lt;&gt;description(viewer, 'displays image').&lt;&gt;visual_style(viewer,  visual_style11).&lt;&gt;inputs(viewer, [required('A')]).&lt;&gt;outputs(viewer, []).&lt;&gt;input_types(viewer, [image]).&lt;&gt;output_types(viewer, []).&lt;&gt;image_name(viewer, '/img/blocks/blocksheet1_13.png').&lt;&gt;prototype_coordinates(viewer, 21, 8).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== viewer ===========&lt;&gt;section(viewer, 'I/O').&lt;&gt;subsection(viewer, 'imaging').&lt;&gt;description(viewer, 'displays image').&lt;&gt;visual_style(viewer,  visual_style11).&lt;&gt;inputs(viewer, [required('A')]).&lt;&gt;outputs(viewer, []).&lt;&gt;input_types(viewer, [image]).&lt;&gt;output_types(viewer, []).&lt;&gt;image_name(viewer, '/img/blocks/blocksheet1_13.png').&lt;&gt;prototype_coordinates(viewer, 21, 8).&lt;&gt;icon_size(viewer, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="30" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5135,6 +5336,12 @@
       <c r="AS30">
         <v>1</v>
       </c>
+      <c r="AZ30">
+        <v>1</v>
+      </c>
+      <c r="BA30">
+        <v>1</v>
+      </c>
       <c r="BB30" t="s">
         <v>281</v>
       </c>
@@ -5146,7 +5353,7 @@
       </c>
       <c r="BE30" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== kernal ===========&lt;&gt;section(kernal, 'I/O').&lt;&gt;subsection(kernal, 'imaging').&lt;&gt;description(kernal, 'kernal UI for defining kernals').&lt;&gt;visual_style(kernal,  visual_style12).&lt;&gt;inputs(kernal, []).&lt;&gt;outputs(kernal, ['O']).&lt;&gt;input_types(kernal, []).&lt;&gt;output_types(kernal, [kernal]).&lt;&gt;image_name(kernal, '/img/blocks/blocksheet1_14.png').&lt;&gt;prototype_coordinates(kernal, 21, 9).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== kernal ===========&lt;&gt;section(kernal, 'I/O').&lt;&gt;subsection(kernal, 'imaging').&lt;&gt;description(kernal, 'kernal UI for defining kernals').&lt;&gt;visual_style(kernal,  visual_style12).&lt;&gt;inputs(kernal, []).&lt;&gt;outputs(kernal, ['O']).&lt;&gt;input_types(kernal, []).&lt;&gt;output_types(kernal, [kernal]).&lt;&gt;image_name(kernal, '/img/blocks/blocksheet1_14.png').&lt;&gt;prototype_coordinates(kernal, 21, 9).&lt;&gt;icon_size(kernal, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="31" spans="2:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5380,6 +5587,12 @@
       <c r="AS32">
         <v>1</v>
       </c>
+      <c r="AZ32">
+        <v>1</v>
+      </c>
+      <c r="BA32">
+        <v>1</v>
+      </c>
       <c r="BB32" t="s">
         <v>282</v>
       </c>
@@ -5391,7 +5604,7 @@
       </c>
       <c r="BE32" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== bodymask ===========&lt;&gt;section(bodymask, 'I/O').&lt;&gt;subsection(bodymask, 'body').&lt;&gt;description(bodymask, 'output is a vector of booleans for joints').&lt;&gt;visual_style(bodymask,  visual_style13).&lt;&gt;inputs(bodymask, []).&lt;&gt;outputs(bodymask, ['O']).&lt;&gt;input_types(bodymask, []).&lt;&gt;output_types(bodymask, [mask]).&lt;&gt;image_name(bodymask, '/img/blocks/blocksheet1_10.png').&lt;&gt;prototype_coordinates(bodymask, 21, 10).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== bodymask ===========&lt;&gt;section(bodymask, 'I/O').&lt;&gt;subsection(bodymask, 'body').&lt;&gt;description(bodymask, 'output is a vector of booleans for joints').&lt;&gt;visual_style(bodymask,  visual_style13).&lt;&gt;inputs(bodymask, []).&lt;&gt;outputs(bodymask, ['O']).&lt;&gt;input_types(bodymask, []).&lt;&gt;output_types(bodymask, [mask]).&lt;&gt;image_name(bodymask, '/img/blocks/blocksheet1_10.png').&lt;&gt;prototype_coordinates(bodymask, 21, 10).&lt;&gt;icon_size(bodymask, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5511,6 +5724,12 @@
       <c r="AS33">
         <v>1</v>
       </c>
+      <c r="AZ33">
+        <v>1</v>
+      </c>
+      <c r="BA33">
+        <v>1</v>
+      </c>
       <c r="BB33" t="s">
         <v>284</v>
       </c>
@@ -5522,7 +5741,7 @@
       </c>
       <c r="BE33" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== bodyposition ===========&lt;&gt;section(bodyposition, 'I/O').&lt;&gt;subsection(bodyposition, 'body').&lt;&gt;description(bodyposition, 'output is a vector of joint positions from physivcal bot').&lt;&gt;visual_style(bodyposition,  normal).&lt;&gt;inputs(bodyposition, []).&lt;&gt;outputs(bodyposition, ['O']).&lt;&gt;input_types(bodyposition, []).&lt;&gt;output_types(bodyposition, [joints]).&lt;&gt;image_name(bodyposition, '/img/blocks/blocksheet1_11.png').&lt;&gt;prototype_coordinates(bodyposition, 21, 11).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== bodyposition ===========&lt;&gt;section(bodyposition, 'I/O').&lt;&gt;subsection(bodyposition, 'body').&lt;&gt;description(bodyposition, 'output is a vector of joint positions from physivcal bot').&lt;&gt;visual_style(bodyposition,  normal).&lt;&gt;inputs(bodyposition, []).&lt;&gt;outputs(bodyposition, ['O']).&lt;&gt;input_types(bodyposition, []).&lt;&gt;output_types(bodyposition, [joints]).&lt;&gt;image_name(bodyposition, '/img/blocks/blocksheet1_11.png').&lt;&gt;prototype_coordinates(bodyposition, 21, 11).&lt;&gt;icon_size(bodyposition, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5642,6 +5861,12 @@
       <c r="AS34">
         <v>1</v>
       </c>
+      <c r="AZ34">
+        <v>1</v>
+      </c>
+      <c r="BA34">
+        <v>1</v>
+      </c>
       <c r="BB34" t="s">
         <v>285</v>
       </c>
@@ -5653,7 +5878,7 @@
       </c>
       <c r="BE34" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== bodypossim ===========&lt;&gt;section(bodypossim, 'I/O').&lt;&gt;subsection(bodypossim, 'body').&lt;&gt;description(bodypossim, 'as per bodyposition but from the simulator').&lt;&gt;visual_style(bodypossim,  normal).&lt;&gt;inputs(bodypossim, []).&lt;&gt;outputs(bodypossim, ['O']).&lt;&gt;input_types(bodypossim, []).&lt;&gt;output_types(bodypossim, [joints]).&lt;&gt;image_name(bodypossim, '/img/blocks/blocksheet1_16.png').&lt;&gt;prototype_coordinates(bodypossim, 21, 12).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== bodypossim ===========&lt;&gt;section(bodypossim, 'I/O').&lt;&gt;subsection(bodypossim, 'body').&lt;&gt;description(bodypossim, 'as per bodyposition but from the simulator').&lt;&gt;visual_style(bodypossim,  normal).&lt;&gt;inputs(bodypossim, []).&lt;&gt;outputs(bodypossim, ['O']).&lt;&gt;input_types(bodypossim, []).&lt;&gt;output_types(bodypossim, [joints]).&lt;&gt;image_name(bodypossim, '/img/blocks/blocksheet1_16.png').&lt;&gt;prototype_coordinates(bodypossim, 21, 12).&lt;&gt;icon_size(bodypossim, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5778,6 +6003,12 @@
       <c r="AS35">
         <v>1</v>
       </c>
+      <c r="AZ35">
+        <v>1</v>
+      </c>
+      <c r="BA35">
+        <v>1</v>
+      </c>
       <c r="BB35" t="s">
         <v>283</v>
       </c>
@@ -5789,7 +6020,7 @@
       </c>
       <c r="BE35" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== motors ===========&lt;&gt;section(motors, 'I/O').&lt;&gt;subsection(motors, 'body').&lt;&gt;description(motors, 'Send channels of vector A matching Mask to robot servos').&lt;&gt;visual_style(motors,  normal).&lt;&gt;inputs(motors, [required('A'), required('Mask')]).&lt;&gt;outputs(motors, []).&lt;&gt;input_types(motors, [joints, jointmask]).&lt;&gt;output_types(motors, []).&lt;&gt;image_name(motors, '/img/blocks/blocksheet1_15.png').&lt;&gt;prototype_coordinates(motors, 21, 13).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== motors ===========&lt;&gt;section(motors, 'I/O').&lt;&gt;subsection(motors, 'body').&lt;&gt;description(motors, 'Send channels of vector A matching Mask to robot servos').&lt;&gt;visual_style(motors,  normal).&lt;&gt;inputs(motors, [required('A'), required('Mask')]).&lt;&gt;outputs(motors, []).&lt;&gt;input_types(motors, [joints, jointmask]).&lt;&gt;output_types(motors, []).&lt;&gt;image_name(motors, '/img/blocks/blocksheet1_15.png').&lt;&gt;prototype_coordinates(motors, 21, 13).&lt;&gt;icon_size(motors, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5914,6 +6145,12 @@
       <c r="AS36">
         <v>1</v>
       </c>
+      <c r="AZ36">
+        <v>1</v>
+      </c>
+      <c r="BA36">
+        <v>1</v>
+      </c>
       <c r="BB36" t="s">
         <v>286</v>
       </c>
@@ -5925,7 +6162,7 @@
       </c>
       <c r="BE36" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== motorsim ===========&lt;&gt;section(motorsim, 'I/O').&lt;&gt;subsection(motorsim, 'body').&lt;&gt;description(motorsim, 'As per motors, but to simulator').&lt;&gt;visual_style(motorsim,  normal).&lt;&gt;inputs(motorsim, [required('A'), required('Mask')]).&lt;&gt;outputs(motorsim, []).&lt;&gt;input_types(motorsim, [joints, jointmask]).&lt;&gt;output_types(motorsim, []).&lt;&gt;image_name(motorsim, '/img/blocks/blocksheet1_17.png').&lt;&gt;prototype_coordinates(motorsim, 21, 14).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== motorsim ===========&lt;&gt;section(motorsim, 'I/O').&lt;&gt;subsection(motorsim, 'body').&lt;&gt;description(motorsim, 'As per motors, but to simulator').&lt;&gt;visual_style(motorsim,  normal).&lt;&gt;inputs(motorsim, [required('A'), required('Mask')]).&lt;&gt;outputs(motorsim, []).&lt;&gt;input_types(motorsim, [joints, jointmask]).&lt;&gt;output_types(motorsim, []).&lt;&gt;image_name(motorsim, '/img/blocks/blocksheet1_17.png').&lt;&gt;prototype_coordinates(motorsim, 21, 14).&lt;&gt;icon_size(motorsim, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6310,7 +6547,7 @@
       </c>
       <c r="BE39" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== drbend ===========&lt;&gt;section(drbend, 'connector').&lt;&gt;subsection(drbend, 'pipe').&lt;&gt;description(drbend, 'bidi pipe connection').&lt;&gt;visual_style(drbend,  visual_style14).&lt;&gt;inputs(drbend, [required('A')]).&lt;&gt;outputs(drbend, ['O']).&lt;&gt;input_types(drbend, [any]).&lt;&gt;output_types(drbend, [any]).&lt;&gt;image_name(drbend, '/img/blocks/blocksheet0-_02.png').&lt;&gt;prototype_coordinates(drbend, 20, 0).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== drbend ===========&lt;&gt;section(drbend, 'connector').&lt;&gt;subsection(drbend, 'pipe').&lt;&gt;description(drbend, 'bidi pipe connection').&lt;&gt;visual_style(drbend,  visual_style14).&lt;&gt;inputs(drbend, [required('A')]).&lt;&gt;outputs(drbend, ['O']).&lt;&gt;input_types(drbend, [any]).&lt;&gt;output_types(drbend, [any]).&lt;&gt;image_name(drbend, '/img/blocks/blocksheet0-_02.png').&lt;&gt;prototype_coordinates(drbend, 20, 0).&lt;&gt;icon_size(drbend, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6467,7 +6704,7 @@
       </c>
       <c r="BE40" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== dlbend ===========&lt;&gt;section(dlbend, 'connector').&lt;&gt;subsection(dlbend, 'pipe').&lt;&gt;description(dlbend, 'bidi pipe connection').&lt;&gt;visual_style(dlbend,  visual_style15).&lt;&gt;inputs(dlbend, [required('A')]).&lt;&gt;outputs(dlbend, ['O']).&lt;&gt;input_types(dlbend, [any]).&lt;&gt;output_types(dlbend, [any]).&lt;&gt;image_name(dlbend, '/img/blocks/blocksheet0-_03.png').&lt;&gt;prototype_coordinates(dlbend, 20, 1).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== dlbend ===========&lt;&gt;section(dlbend, 'connector').&lt;&gt;subsection(dlbend, 'pipe').&lt;&gt;description(dlbend, 'bidi pipe connection').&lt;&gt;visual_style(dlbend,  visual_style15).&lt;&gt;inputs(dlbend, [required('A')]).&lt;&gt;outputs(dlbend, ['O']).&lt;&gt;input_types(dlbend, [any]).&lt;&gt;output_types(dlbend, [any]).&lt;&gt;image_name(dlbend, '/img/blocks/blocksheet0-_03.png').&lt;&gt;prototype_coordinates(dlbend, 20, 1).&lt;&gt;icon_size(dlbend, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6625,7 +6862,7 @@
       </c>
       <c r="BE41" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== horpipe ===========&lt;&gt;section(horpipe, 'connector').&lt;&gt;subsection(horpipe, 'pipe').&lt;&gt;description(horpipe, 'bidi pipe connection').&lt;&gt;visual_style(horpipe,  visual_style16).&lt;&gt;inputs(horpipe, [required('A')]).&lt;&gt;outputs(horpipe, ['O']).&lt;&gt;input_types(horpipe, [any]).&lt;&gt;output_types(horpipe, [any]).&lt;&gt;image_name(horpipe, '/img/blocks/blocksheet0-_04.png').&lt;&gt;prototype_coordinates(horpipe, 20, 2).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== horpipe ===========&lt;&gt;section(horpipe, 'connector').&lt;&gt;subsection(horpipe, 'pipe').&lt;&gt;description(horpipe, 'bidi pipe connection').&lt;&gt;visual_style(horpipe,  visual_style16).&lt;&gt;inputs(horpipe, [required('A')]).&lt;&gt;outputs(horpipe, ['O']).&lt;&gt;input_types(horpipe, [any]).&lt;&gt;output_types(horpipe, [any]).&lt;&gt;image_name(horpipe, '/img/blocks/blocksheet0-_04.png').&lt;&gt;prototype_coordinates(horpipe, 20, 2).&lt;&gt;icon_size(horpipe, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="42" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6794,7 +7031,7 @@
       </c>
       <c r="BE42" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== cross ===========&lt;&gt;section(cross, 'connector').&lt;&gt;subsection(cross, 'pipe').&lt;&gt;description(cross, 'bidi pipe connection').&lt;&gt;visual_style(cross,  visual_style17).&lt;&gt;inputs(cross, [required('A'), required('B')]).&lt;&gt;outputs(cross, ['OA', 'OB']).&lt;&gt;input_types(cross, [any, any]).&lt;&gt;output_types(cross, [any, any]).&lt;&gt;image_name(cross, '/img/blocks/blocksheet0-_05.png').&lt;&gt;prototype_coordinates(cross, 20, 3).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== cross ===========&lt;&gt;section(cross, 'connector').&lt;&gt;subsection(cross, 'pipe').&lt;&gt;description(cross, 'bidi pipe connection').&lt;&gt;visual_style(cross,  visual_style17).&lt;&gt;inputs(cross, [required('A'), required('B')]).&lt;&gt;outputs(cross, ['OA', 'OB']).&lt;&gt;input_types(cross, [any, any]).&lt;&gt;output_types(cross, [any, any]).&lt;&gt;image_name(cross, '/img/blocks/blocksheet0-_05.png').&lt;&gt;prototype_coordinates(cross, 20, 3).&lt;&gt;icon_size(cross, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -6952,7 +7189,7 @@
       </c>
       <c r="BE43" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== urbend ===========&lt;&gt;section(urbend, 'connector').&lt;&gt;subsection(urbend, 'pipe').&lt;&gt;description(urbend, 'bidi pipe connection').&lt;&gt;visual_style(urbend,  visual_style18).&lt;&gt;inputs(urbend, [required('A')]).&lt;&gt;outputs(urbend, ['O']).&lt;&gt;input_types(urbend, [any]).&lt;&gt;output_types(urbend, [any]).&lt;&gt;image_name(urbend, '/img/blocks/blocksheet0-_14.png').&lt;&gt;prototype_coordinates(urbend, 20, 4).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== urbend ===========&lt;&gt;section(urbend, 'connector').&lt;&gt;subsection(urbend, 'pipe').&lt;&gt;description(urbend, 'bidi pipe connection').&lt;&gt;visual_style(urbend,  visual_style18).&lt;&gt;inputs(urbend, [required('A')]).&lt;&gt;outputs(urbend, ['O']).&lt;&gt;input_types(urbend, [any]).&lt;&gt;output_types(urbend, [any]).&lt;&gt;image_name(urbend, '/img/blocks/blocksheet0-_14.png').&lt;&gt;prototype_coordinates(urbend, 20, 4).&lt;&gt;icon_size(urbend, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7110,7 +7347,7 @@
       </c>
       <c r="BE44" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== ulbend ===========&lt;&gt;section(ulbend, 'connector').&lt;&gt;subsection(ulbend, 'pipe').&lt;&gt;description(ulbend, 'bidi pipe connection').&lt;&gt;visual_style(ulbend,  visual_style19).&lt;&gt;inputs(ulbend, [required('A')]).&lt;&gt;outputs(ulbend, ['O']).&lt;&gt;input_types(ulbend, [any]).&lt;&gt;output_types(ulbend, [any]).&lt;&gt;image_name(ulbend, '/img/blocks/blocksheet0-_11.png').&lt;&gt;prototype_coordinates(ulbend, 20, 5).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== ulbend ===========&lt;&gt;section(ulbend, 'connector').&lt;&gt;subsection(ulbend, 'pipe').&lt;&gt;description(ulbend, 'bidi pipe connection').&lt;&gt;visual_style(ulbend,  visual_style19).&lt;&gt;inputs(ulbend, [required('A')]).&lt;&gt;outputs(ulbend, ['O']).&lt;&gt;input_types(ulbend, [any]).&lt;&gt;output_types(ulbend, [any]).&lt;&gt;image_name(ulbend, '/img/blocks/blocksheet0-_11.png').&lt;&gt;prototype_coordinates(ulbend, 20, 5).&lt;&gt;icon_size(ulbend, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7280,7 +7517,7 @@
       </c>
       <c r="BE45" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== distributor ===========&lt;&gt;section(distributor, 'connector').&lt;&gt;subsection(distributor, 'pipe').&lt;&gt;description(distributor, 'bidi pipe connection').&lt;&gt;visual_style(distributor,  visual_style20).&lt;&gt;inputs(distributor, [required('A')]).&lt;&gt;outputs(distributor, ['OA', 'OB', 'OC']).&lt;&gt;input_types(distributor, [any]).&lt;&gt;output_types(distributor, [any, any, any]).&lt;&gt;image_name(distributor, '/img/blocks/blocksheet0-_09.png').&lt;&gt;prototype_coordinates(distributor, 20, 6).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== distributor ===========&lt;&gt;section(distributor, 'connector').&lt;&gt;subsection(distributor, 'pipe').&lt;&gt;description(distributor, 'bidi pipe connection').&lt;&gt;visual_style(distributor,  visual_style20).&lt;&gt;inputs(distributor, [required('A')]).&lt;&gt;outputs(distributor, ['OA', 'OB', 'OC']).&lt;&gt;input_types(distributor, [any]).&lt;&gt;output_types(distributor, [any, any, any]).&lt;&gt;image_name(distributor, '/img/blocks/blocksheet0-_09.png').&lt;&gt;prototype_coordinates(distributor, 20, 6).&lt;&gt;icon_size(distributor, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -7405,6 +7642,12 @@
         <f t="shared" si="50"/>
         <v>[any]</v>
       </c>
+      <c r="AZ46">
+        <v>1</v>
+      </c>
+      <c r="BA46">
+        <v>1</v>
+      </c>
       <c r="BB46" t="s">
         <v>287</v>
       </c>
@@ -7416,7 +7659,7 @@
       </c>
       <c r="BE46" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== vertpipe ===========&lt;&gt;section(vertpipe, 'connector').&lt;&gt;subsection(vertpipe, 'pipe').&lt;&gt;description(vertpipe, 'bidi pipe connection').&lt;&gt;visual_style(vertpipe,  visual_style21).&lt;&gt;inputs(vertpipe, [required('A')]).&lt;&gt;outputs(vertpipe, ['OA']).&lt;&gt;input_types(vertpipe, [any]).&lt;&gt;output_types(vertpipe, [any]).&lt;&gt;image_name(vertpipe, '/img/blocks/blocksheet0-_08.png').&lt;&gt;prototype_coordinates(vertpipe, 20, 7).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== vertpipe ===========&lt;&gt;section(vertpipe, 'connector').&lt;&gt;subsection(vertpipe, 'pipe').&lt;&gt;description(vertpipe, 'bidi pipe connection').&lt;&gt;visual_style(vertpipe,  visual_style21).&lt;&gt;inputs(vertpipe, [required('A')]).&lt;&gt;outputs(vertpipe, ['OA']).&lt;&gt;input_types(vertpipe, [any]).&lt;&gt;output_types(vertpipe, [any]).&lt;&gt;image_name(vertpipe, '/img/blocks/blocksheet0-_08.png').&lt;&gt;prototype_coordinates(vertpipe, 20, 7).&lt;&gt;icon_size(vertpipe, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9847,7 +10090,7 @@
         <v/>
       </c>
       <c r="BE68" t="str">
-        <f t="shared" ref="BE68:BE109" si="64">AH68&amp;IF(OR(ISBLANK(E68),ISBLANK(BC68)), "", "prototype_coordinates("&amp;E68&amp;", "&amp;BC68&amp;", "&amp;BD68&amp;").&lt;&gt;")</f>
+        <f t="shared" ref="BE68:BE109" si="64">AH68&amp;IF(OR(ISBLANK(E68),ISBLANK(BC68)), "", "prototype_coordinates("&amp;E68&amp;", "&amp;BC68&amp;", "&amp;BD68&amp;").&lt;&gt;icon_size("&amp;E68&amp;", "&amp;AZ68&amp;", "&amp;BA68&amp;").&lt;&gt;")</f>
         <v/>
       </c>
     </row>
@@ -12987,4 +13230,2580 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC117"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="7050" ySplit="540" topLeftCell="W1" activePane="bottomRight"/>
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
+      <selection pane="topRight" activeCell="AD1" sqref="AD1:AD1048576"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomRight" activeCell="Y2" sqref="Y2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="17.140625" style="14"/>
+    <col min="4" max="4" width="8.5703125" style="16" customWidth="1"/>
+    <col min="5" max="7" width="8.5703125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="12" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="14" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="14" customWidth="1"/>
+    <col min="11" max="11" width="10" style="14" customWidth="1"/>
+    <col min="12" max="13" width="5.85546875" style="14" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" style="17" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" style="14" customWidth="1"/>
+    <col min="16" max="17" width="10.7109375" style="14" customWidth="1"/>
+    <col min="18" max="18" width="46.140625" style="15" customWidth="1"/>
+    <col min="19" max="19" width="25.7109375" style="14" customWidth="1"/>
+    <col min="20" max="20" width="17.140625" style="14"/>
+    <col min="21" max="21" width="23.7109375" style="14" customWidth="1"/>
+    <col min="22" max="22" width="87.7109375" style="14" customWidth="1"/>
+    <col min="23" max="26" width="17.140625" style="14"/>
+    <col min="27" max="27" width="21.28515625" style="14" customWidth="1"/>
+    <col min="28" max="16384" width="17.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="X1" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="AA1" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="AB1" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="AC1" s="25"/>
+    </row>
+    <row r="2" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="16"/>
+    </row>
+    <row r="3" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="K3" s="18"/>
+      <c r="L3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="V3" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y3" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="AB3" s="14">
+        <v>22</v>
+      </c>
+      <c r="AC3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="K4" s="18"/>
+      <c r="L4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="V4" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y4" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="AB4" s="14">
+        <v>22</v>
+      </c>
+      <c r="AC4" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="U5" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="AB5" s="14">
+        <v>22</v>
+      </c>
+      <c r="AC5" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="16"/>
+    </row>
+    <row r="7" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="U7" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="AB7" s="14">
+        <v>22</v>
+      </c>
+      <c r="AC7" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="R8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="W8" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="AB8" s="14">
+        <v>22</v>
+      </c>
+      <c r="AC8" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="16"/>
+      <c r="R9" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="S9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="W9" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="AB9" s="14">
+        <v>22</v>
+      </c>
+      <c r="AC9" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="16"/>
+    </row>
+    <row r="11" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="R11" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="U11" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="14">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="AB11" s="14">
+        <v>23</v>
+      </c>
+      <c r="AC11" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="16"/>
+    </row>
+    <row r="13" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="17"/>
+      <c r="H13" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O13" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="R13" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="U13" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="AB13" s="14">
+        <v>23</v>
+      </c>
+      <c r="AC13" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="16"/>
+    </row>
+    <row r="15" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="16"/>
+    </row>
+    <row r="16" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="17"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="R16" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="S16" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="U16" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="AB16" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC16" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="R17" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="S17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="U17" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="AB17" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC17" s="14">
+        <f>AC16+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O18" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="R18" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="S18" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="U18" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="AB18" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC18" s="14">
+        <f>AC17+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="16"/>
+    </row>
+    <row r="20" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="17"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O20" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="R20" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="U20" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="AB20" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC20" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="17"/>
+      <c r="H21" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="16"/>
+      <c r="R21" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="S21" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="U21" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="AB21" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC21" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="17"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="16"/>
+    </row>
+    <row r="23" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="17"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="P23" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="R23" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="S23" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="U23" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="AB23" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC23" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" s="17"/>
+      <c r="H24" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="M24" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="O24" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="P24" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R24" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="U24" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="14">
+        <v>2</v>
+      </c>
+      <c r="Z24" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="AB24" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC24" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="17"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="M25" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="O25" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="P25" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="R25" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="S25" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="U25" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C26" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="17"/>
+      <c r="H26" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="16"/>
+      <c r="R26" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="S26" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="U26" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="17"/>
+      <c r="H27" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="16"/>
+      <c r="R27" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="S27" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="U27" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="AB27" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC27" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C28" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="G28" s="17"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O28" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R28" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="S28" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="U28" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="17"/>
+      <c r="H29" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="16"/>
+      <c r="R29" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="S29" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="U29" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y29" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="AB29" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC29" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C30" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="17"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O30" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="R30" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="S30" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="U30" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z30" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="AB30" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC30" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G31" s="17"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="16"/>
+    </row>
+    <row r="32" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G32" s="17"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O32" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="R32" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="S32" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="U32" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y32" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z32" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA32" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="AB32" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC32" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G33" s="17"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O33" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="R33" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="U33" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="AB33" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC33" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G34" s="17"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O34" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="R34" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="U34" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y34" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="AB34" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC34" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G35" s="17"/>
+      <c r="H35" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="16"/>
+      <c r="R35" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="U35" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y35" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z35" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA35" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="AB35" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC35" s="14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G36" s="17"/>
+      <c r="H36" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="I36" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="16"/>
+      <c r="R36" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="U36" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y36" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA36" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="AB36" s="14">
+        <v>21</v>
+      </c>
+      <c r="AC36" s="14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="G37" s="17"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="16"/>
+    </row>
+    <row r="38" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="G38" s="17"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="16"/>
+    </row>
+    <row r="39" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="17"/>
+      <c r="H39" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O39" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="R39" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="S39" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="V39" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="W39" s="14">
+        <v>1</v>
+      </c>
+      <c r="X39" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z39" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA39" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="AB39" s="14">
+        <v>20</v>
+      </c>
+      <c r="AC39" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="17"/>
+      <c r="H40" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O40" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="R40" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="S40" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="W40" s="14">
+        <v>1</v>
+      </c>
+      <c r="X40" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y40" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA40" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="AB40" s="14">
+        <v>20</v>
+      </c>
+      <c r="AC40" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="17"/>
+      <c r="H41" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O41" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="R41" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="S41" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="W41" s="14">
+        <v>1</v>
+      </c>
+      <c r="X41" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y41" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="AB41" s="14">
+        <v>20</v>
+      </c>
+      <c r="AC41" s="14">
+        <f>AC40+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="17"/>
+      <c r="H42" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="I42" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="M42" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="O42" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="P42" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="R42" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="S42" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="W42" s="14">
+        <v>1</v>
+      </c>
+      <c r="X42" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y42" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z42" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA42" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="AB42" s="14">
+        <v>20</v>
+      </c>
+      <c r="AC42" s="14">
+        <f t="shared" ref="AC42:AC45" si="0">AC41+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="17"/>
+      <c r="H43" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O43" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="R43" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="S43" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="W43" s="14">
+        <v>1</v>
+      </c>
+      <c r="X43" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y43" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z43" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA43" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="AB43" s="14">
+        <v>20</v>
+      </c>
+      <c r="AC43" s="14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C44" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="17"/>
+      <c r="H44" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O44" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="R44" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="S44" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="W44" s="14">
+        <v>1</v>
+      </c>
+      <c r="X44" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y44" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z44" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA44" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="AB44" s="14">
+        <v>20</v>
+      </c>
+      <c r="AC44" s="14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="17"/>
+      <c r="H45" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="M45" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="N45" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="O45" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="P45" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q45" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="R45" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="S45" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="W45" s="14">
+        <v>1</v>
+      </c>
+      <c r="X45" s="14">
+        <v>1</v>
+      </c>
+      <c r="Y45" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA45" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="AB45" s="14">
+        <v>20</v>
+      </c>
+      <c r="AC45" s="14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="17"/>
+      <c r="H46" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="O46" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="R46" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="S46" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y46" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z46" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA46" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="AB46" s="14">
+        <v>20</v>
+      </c>
+      <c r="AC46" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G47" s="17"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="16"/>
+    </row>
+    <row r="48" spans="1:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G48" s="17"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="16"/>
+    </row>
+    <row r="49" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C49" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G49" s="17"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O49" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="R49" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="V49" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C50" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="G50" s="17"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O50" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="R50" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="V50" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G51" s="17"/>
+      <c r="H51" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I51" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O51" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="R51" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="V51" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="52" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C52" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="17"/>
+      <c r="H52" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O52" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="R52" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="V52" s="14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="53" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C53" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="17"/>
+      <c r="H53" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O53" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="R53" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="17"/>
+      <c r="H54" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="I54" s="18"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O54" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="R54" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C55" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G55" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="H55" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="I55" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="J55" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="K55" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="L55" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O55" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="R55" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="17"/>
+      <c r="H56" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I56" s="18"/>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="M56" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="N56" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="O56" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="P56" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q56" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="R56" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C57" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="G57" s="17"/>
+      <c r="H57" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I57" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O57" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="R57" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="S57" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C58" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="G58" s="17"/>
+      <c r="H58" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I58" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J58" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="K58" s="18"/>
+      <c r="L58" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O58" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="R58" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C59" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G59" s="17"/>
+      <c r="H59" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I59" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="J59" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="K59" s="18"/>
+      <c r="L59" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O59" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="R59" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C60" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="G60" s="17"/>
+      <c r="H60" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I60" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O60" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="61" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G61" s="17"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="16"/>
+    </row>
+    <row r="62" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C62" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D62" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="17"/>
+      <c r="H62" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="I62" s="18"/>
+      <c r="J62" s="18"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="O62" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="R62" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="2:22" s="19" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C63" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63" s="21"/>
+      <c r="H63" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="L63" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="N63" s="21"/>
+      <c r="O63" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="R63" s="22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="2:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G64" s="17"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
+      <c r="J64" s="18"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="16"/>
+    </row>
+    <row r="65" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G65" s="17"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="16"/>
+    </row>
+    <row r="66" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G66" s="17"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18"/>
+      <c r="J66" s="18"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="16"/>
+    </row>
+    <row r="67" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G67" s="17"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+      <c r="K67" s="18"/>
+      <c r="L67" s="16"/>
+    </row>
+    <row r="68" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G68" s="17"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+      <c r="J68" s="18"/>
+      <c r="K68" s="18"/>
+      <c r="L68" s="16"/>
+    </row>
+    <row r="69" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G69" s="17"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+      <c r="J69" s="18"/>
+      <c r="K69" s="18"/>
+      <c r="L69" s="16"/>
+    </row>
+    <row r="70" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G70" s="17"/>
+      <c r="H70" s="18"/>
+      <c r="I70" s="18"/>
+      <c r="J70" s="18"/>
+      <c r="K70" s="18"/>
+      <c r="L70" s="16"/>
+    </row>
+    <row r="71" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G71" s="17"/>
+      <c r="H71" s="18"/>
+      <c r="I71" s="18"/>
+      <c r="J71" s="18"/>
+      <c r="K71" s="18"/>
+      <c r="L71" s="16"/>
+    </row>
+    <row r="72" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G72" s="17"/>
+      <c r="H72" s="18"/>
+      <c r="I72" s="18"/>
+      <c r="J72" s="18"/>
+      <c r="K72" s="18"/>
+      <c r="L72" s="16"/>
+    </row>
+    <row r="73" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G73" s="17"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
+      <c r="J73" s="18"/>
+      <c r="K73" s="18"/>
+      <c r="L73" s="16"/>
+    </row>
+    <row r="74" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G74" s="17"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+      <c r="J74" s="18"/>
+      <c r="K74" s="18"/>
+      <c r="L74" s="16"/>
+    </row>
+    <row r="75" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G75" s="17"/>
+      <c r="H75" s="18"/>
+      <c r="I75" s="18"/>
+      <c r="J75" s="18"/>
+      <c r="K75" s="18"/>
+      <c r="L75" s="16"/>
+    </row>
+    <row r="76" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G76" s="17"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+      <c r="J76" s="18"/>
+      <c r="K76" s="18"/>
+      <c r="L76" s="16"/>
+    </row>
+    <row r="77" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G77" s="17"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="18"/>
+      <c r="J77" s="18"/>
+      <c r="K77" s="18"/>
+      <c r="L77" s="16"/>
+    </row>
+    <row r="78" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G78" s="17"/>
+      <c r="H78" s="18"/>
+      <c r="I78" s="18"/>
+      <c r="J78" s="18"/>
+      <c r="K78" s="18"/>
+      <c r="L78" s="16"/>
+    </row>
+    <row r="79" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G79" s="17"/>
+      <c r="H79" s="18"/>
+      <c r="I79" s="18"/>
+      <c r="J79" s="18"/>
+      <c r="K79" s="18"/>
+      <c r="L79" s="16"/>
+    </row>
+    <row r="80" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G80" s="17"/>
+      <c r="H80" s="18"/>
+      <c r="I80" s="18"/>
+      <c r="J80" s="18"/>
+      <c r="K80" s="18"/>
+      <c r="L80" s="16"/>
+    </row>
+    <row r="81" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G81" s="17"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="18"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="18"/>
+      <c r="L81" s="16"/>
+    </row>
+    <row r="82" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G82" s="17"/>
+      <c r="H82" s="18"/>
+      <c r="I82" s="18"/>
+      <c r="J82" s="18"/>
+      <c r="K82" s="18"/>
+      <c r="L82" s="16"/>
+    </row>
+    <row r="83" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G83" s="17"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+      <c r="J83" s="18"/>
+      <c r="K83" s="18"/>
+      <c r="L83" s="16"/>
+    </row>
+    <row r="84" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G84" s="17"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
+      <c r="J84" s="18"/>
+      <c r="K84" s="18"/>
+      <c r="L84" s="16"/>
+    </row>
+    <row r="85" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G85" s="17"/>
+      <c r="H85" s="18"/>
+      <c r="I85" s="18"/>
+      <c r="J85" s="18"/>
+      <c r="K85" s="18"/>
+      <c r="L85" s="16"/>
+    </row>
+    <row r="86" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G86" s="17"/>
+      <c r="H86" s="18"/>
+      <c r="I86" s="18"/>
+      <c r="J86" s="18"/>
+      <c r="K86" s="18"/>
+      <c r="L86" s="16"/>
+    </row>
+    <row r="87" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G87" s="17"/>
+      <c r="H87" s="18"/>
+      <c r="I87" s="18"/>
+      <c r="J87" s="18"/>
+      <c r="K87" s="18"/>
+      <c r="L87" s="16"/>
+    </row>
+    <row r="88" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G88" s="17"/>
+      <c r="H88" s="18"/>
+      <c r="I88" s="18"/>
+      <c r="J88" s="18"/>
+      <c r="K88" s="18"/>
+      <c r="L88" s="16"/>
+    </row>
+    <row r="89" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G89" s="17"/>
+      <c r="H89" s="18"/>
+      <c r="I89" s="18"/>
+      <c r="J89" s="18"/>
+      <c r="K89" s="18"/>
+      <c r="L89" s="16"/>
+    </row>
+    <row r="90" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G90" s="17"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
+      <c r="J90" s="18"/>
+      <c r="K90" s="18"/>
+      <c r="L90" s="16"/>
+    </row>
+    <row r="91" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G91" s="17"/>
+      <c r="H91" s="18"/>
+      <c r="I91" s="18"/>
+      <c r="J91" s="18"/>
+      <c r="K91" s="18"/>
+      <c r="L91" s="16"/>
+    </row>
+    <row r="92" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G92" s="17"/>
+      <c r="H92" s="18"/>
+      <c r="I92" s="18"/>
+      <c r="J92" s="18"/>
+      <c r="K92" s="18"/>
+      <c r="L92" s="16"/>
+    </row>
+    <row r="93" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G93" s="17"/>
+      <c r="H93" s="18"/>
+      <c r="I93" s="18"/>
+      <c r="J93" s="18"/>
+      <c r="K93" s="18"/>
+      <c r="L93" s="16"/>
+    </row>
+    <row r="94" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G94" s="17"/>
+      <c r="H94" s="18"/>
+      <c r="I94" s="18"/>
+      <c r="J94" s="18"/>
+      <c r="K94" s="18"/>
+      <c r="L94" s="16"/>
+    </row>
+    <row r="95" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G95" s="17"/>
+      <c r="H95" s="18"/>
+      <c r="I95" s="18"/>
+      <c r="J95" s="18"/>
+      <c r="K95" s="18"/>
+      <c r="L95" s="16"/>
+    </row>
+    <row r="96" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G96" s="17"/>
+      <c r="H96" s="18"/>
+      <c r="I96" s="18"/>
+      <c r="J96" s="18"/>
+      <c r="K96" s="18"/>
+      <c r="L96" s="16"/>
+    </row>
+    <row r="97" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G97" s="17"/>
+      <c r="H97" s="18"/>
+      <c r="I97" s="18"/>
+      <c r="J97" s="18"/>
+      <c r="K97" s="18"/>
+      <c r="L97" s="16"/>
+    </row>
+    <row r="98" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G98" s="17"/>
+      <c r="H98" s="18"/>
+      <c r="I98" s="18"/>
+      <c r="J98" s="18"/>
+      <c r="K98" s="18"/>
+      <c r="L98" s="16"/>
+    </row>
+    <row r="99" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G99" s="17"/>
+      <c r="H99" s="18"/>
+      <c r="I99" s="18"/>
+      <c r="J99" s="18"/>
+      <c r="K99" s="18"/>
+      <c r="L99" s="16"/>
+    </row>
+    <row r="100" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G100" s="17"/>
+      <c r="H100" s="18"/>
+      <c r="I100" s="18"/>
+      <c r="J100" s="18"/>
+      <c r="K100" s="18"/>
+      <c r="L100" s="16"/>
+    </row>
+    <row r="101" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G101" s="17"/>
+      <c r="H101" s="18"/>
+      <c r="I101" s="18"/>
+      <c r="J101" s="18"/>
+      <c r="K101" s="18"/>
+      <c r="L101" s="16"/>
+    </row>
+    <row r="102" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G102" s="17"/>
+      <c r="H102" s="18"/>
+      <c r="I102" s="18"/>
+      <c r="J102" s="18"/>
+      <c r="K102" s="18"/>
+      <c r="L102" s="16"/>
+    </row>
+    <row r="103" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G103" s="17"/>
+      <c r="H103" s="18"/>
+      <c r="I103" s="18"/>
+      <c r="J103" s="18"/>
+      <c r="K103" s="18"/>
+      <c r="L103" s="16"/>
+    </row>
+    <row r="104" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G104" s="17"/>
+      <c r="H104" s="18"/>
+      <c r="I104" s="18"/>
+      <c r="J104" s="18"/>
+      <c r="K104" s="18"/>
+      <c r="L104" s="16"/>
+    </row>
+    <row r="105" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G105" s="17"/>
+      <c r="H105" s="18"/>
+      <c r="I105" s="18"/>
+      <c r="J105" s="18"/>
+      <c r="K105" s="18"/>
+      <c r="L105" s="16"/>
+    </row>
+    <row r="106" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G106" s="17"/>
+      <c r="H106" s="18"/>
+      <c r="I106" s="18"/>
+      <c r="J106" s="18"/>
+      <c r="K106" s="18"/>
+      <c r="L106" s="16"/>
+    </row>
+    <row r="107" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G107" s="17"/>
+      <c r="H107" s="18"/>
+      <c r="I107" s="18"/>
+      <c r="J107" s="18"/>
+      <c r="K107" s="18"/>
+      <c r="L107" s="16"/>
+    </row>
+    <row r="108" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G108" s="17"/>
+      <c r="H108" s="18"/>
+      <c r="I108" s="18"/>
+      <c r="J108" s="18"/>
+      <c r="K108" s="18"/>
+      <c r="L108" s="16"/>
+    </row>
+    <row r="109" spans="7:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G109" s="17"/>
+      <c r="H109" s="18"/>
+      <c r="I109" s="18"/>
+      <c r="J109" s="18"/>
+      <c r="K109" s="18"/>
+      <c r="L109" s="16"/>
+    </row>
+    <row r="110" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G110" s="17"/>
+      <c r="H110" s="18"/>
+      <c r="I110" s="18"/>
+      <c r="J110" s="18"/>
+      <c r="K110" s="18"/>
+      <c r="L110" s="16"/>
+    </row>
+    <row r="111" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G111" s="17"/>
+      <c r="H111" s="18"/>
+      <c r="I111" s="18"/>
+      <c r="J111" s="18"/>
+      <c r="K111" s="18"/>
+      <c r="L111" s="16"/>
+    </row>
+    <row r="112" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G112" s="17"/>
+      <c r="H112" s="18"/>
+      <c r="I112" s="18"/>
+      <c r="J112" s="18"/>
+      <c r="K112" s="18"/>
+      <c r="L112" s="16"/>
+    </row>
+    <row r="113" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G113" s="17"/>
+      <c r="H113" s="18"/>
+      <c r="I113" s="18"/>
+      <c r="J113" s="18"/>
+      <c r="K113" s="18"/>
+      <c r="L113" s="16"/>
+    </row>
+    <row r="114" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G114" s="17"/>
+      <c r="H114" s="18"/>
+      <c r="I114" s="18"/>
+      <c r="J114" s="18"/>
+      <c r="K114" s="18"/>
+      <c r="L114" s="16"/>
+    </row>
+    <row r="115" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G115" s="17"/>
+      <c r="H115" s="18"/>
+      <c r="I115" s="18"/>
+      <c r="J115" s="18"/>
+      <c r="K115" s="18"/>
+      <c r="L115" s="16"/>
+    </row>
+    <row r="116" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G116" s="17"/>
+      <c r="H116" s="18"/>
+      <c r="I116" s="18"/>
+      <c r="J116" s="18"/>
+      <c r="K116" s="18"/>
+      <c r="L116" s="16"/>
+    </row>
+    <row r="117" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G117" s="17"/>
+      <c r="H117" s="18"/>
+      <c r="I117" s="18"/>
+      <c r="J117" s="18"/>
+      <c r="K117" s="18"/>
+      <c r="L117" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="AB1:AC1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
oops - hadn't saved the SS
</commit_message>
<xml_diff>
--- a/doc/flo/Blocks.xlsx
+++ b/doc/flo/Blocks.xlsx
@@ -1413,11 +1413,11 @@
   <dimension ref="A1:BE117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="9000" ySplit="540" topLeftCell="BC1" activePane="bottomRight"/>
+      <pane xSplit="9000" ySplit="540" topLeftCell="AH35" activePane="bottomRight"/>
       <selection activeCell="AH1" sqref="AH1"/>
       <selection pane="topRight" activeCell="BE1" sqref="BE1"/>
       <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
-      <selection pane="bottomRight" activeCell="BE2" sqref="BE2"/>
+      <selection pane="bottomRight" activeCell="AH58" sqref="AH58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
some java generation work on flo
</commit_message>
<xml_diff>
--- a/doc/flo/Blocks.xlsx
+++ b/doc/flo/Blocks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="555" windowWidth="12135" windowHeight="7770" tabRatio="842"/>
+    <workbookView xWindow="270" yWindow="555" windowWidth="12135" windowHeight="7350" tabRatio="842"/>
   </bookViews>
   <sheets>
     <sheet name="BlockTypes" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="311">
   <si>
     <t>Block Types</t>
   </si>
@@ -920,6 +920,36 @@
   </si>
   <si>
     <t>takes the channel values from whichever image has R+G+B greatest</t>
+  </si>
+  <si>
+    <t>% = FloFlipFlop.newFlipFlop();</t>
+  </si>
+  <si>
+    <t>FloRT.if($Cond, $A, $B, #O);</t>
+  </si>
+  <si>
+    <t>%.pulse(#O);</t>
+  </si>
+  <si>
+    <t>FloRT.isolate($A, $Default, #O);</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>% = FloInput($Name);</t>
+  </si>
+  <si>
+    <t>FloRT.input(%, #O);</t>
+  </si>
+  <si>
+    <t>% = FloOutput($Name);</t>
+  </si>
+  <si>
+    <t>FloRT.output($A, %, $Name);</t>
+  </si>
+  <si>
+    <t>Formula</t>
   </si>
 </sst>
 </file>
@@ -1427,12 +1457,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="9000" ySplit="540" topLeftCell="AH46" activePane="bottomLeft"/>
-      <selection activeCell="AH1" sqref="AH1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="11835" ySplit="495" topLeftCell="AS1" activePane="bottomLeft"/>
+      <selection activeCell="AT43" sqref="AT43"/>
       <selection pane="topRight" activeCell="BE1" sqref="BE1"/>
-      <selection pane="bottomLeft" activeCell="T67" sqref="T67"/>
-      <selection pane="bottomRight" activeCell="AH58" sqref="AH58"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="AS11" sqref="AS11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1463,7 +1493,7 @@
     <col min="40" max="40" width="8.5703125" customWidth="1"/>
     <col min="41" max="41" width="9.42578125" style="11" customWidth="1"/>
     <col min="42" max="42" width="24" customWidth="1"/>
-    <col min="45" max="45" width="23.7109375" customWidth="1"/>
+    <col min="45" max="45" width="29.28515625" customWidth="1"/>
     <col min="46" max="46" width="87.7109375" customWidth="1"/>
     <col min="54" max="54" width="21.28515625" customWidth="1"/>
     <col min="57" max="57" width="41.28515625" customWidth="1"/>
@@ -1687,7 +1717,7 @@
         <v>[object]</v>
       </c>
       <c r="AT3" t="s">
-        <v>170</v>
+        <v>302</v>
       </c>
       <c r="AW3">
         <v>0</v>
@@ -1848,7 +1878,7 @@
         <v>[object]</v>
       </c>
       <c r="AT4" t="s">
-        <v>167</v>
+        <v>302</v>
       </c>
       <c r="AW4">
         <v>0</v>
@@ -2003,8 +2033,11 @@
         <f t="shared" si="23"/>
         <v>[int]</v>
       </c>
-      <c r="AS5">
-        <v>1</v>
+      <c r="AS5" t="s">
+        <v>301</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>303</v>
       </c>
       <c r="BB5" t="s">
         <v>272</v>
@@ -2255,8 +2288,8 @@
         <f t="shared" si="23"/>
         <v>[object]</v>
       </c>
-      <c r="AS7">
-        <v>1</v>
+      <c r="AT7" t="s">
+        <v>304</v>
       </c>
       <c r="AW7">
         <v>0</v>
@@ -2299,8 +2332,13 @@
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F8" s="2" t="s">
+        <v>305</v>
+      </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="10"/>
+      <c r="J8" s="10" t="s">
+        <v>162</v>
+      </c>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -2318,7 +2356,7 @@
       </c>
       <c r="V8" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>[</v>
+        <v>[required('Name')</v>
       </c>
       <c r="W8" s="9" t="str">
         <f t="shared" si="4"/>
@@ -2334,7 +2372,7 @@
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="7"/>
-        <v>[]</v>
+        <v>[required('Name')]</v>
       </c>
       <c r="AA8" s="1" t="str">
         <f t="shared" si="8"/>
@@ -2366,11 +2404,11 @@
       </c>
       <c r="AH8" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== inputparam ===========&lt;&gt;section(inputparam, 'Editor Support').&lt;&gt;subsection(inputparam, 'Editor Support').&lt;&gt;description(inputparam, 'used when defining new blocks').&lt;&gt;visual_style(inputparam,  visual_style0).&lt;&gt;inputs(inputparam, []).&lt;&gt;outputs(inputparam, ['O']).&lt;&gt;input_types(inputparam, []).&lt;&gt;output_types(inputparam, [object]).&lt;&gt;image_name(inputparam, '/img/blocks/blocksheet0-_15.png').&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== inputparam ===========&lt;&gt;section(inputparam, 'Editor Support').&lt;&gt;subsection(inputparam, 'Editor Support').&lt;&gt;description(inputparam, 'used when defining new blocks').&lt;&gt;visual_style(inputparam,  visual_style0).&lt;&gt;inputs(inputparam, [required('Name')]).&lt;&gt;outputs(inputparam, ['O']).&lt;&gt;input_types(inputparam, [string]).&lt;&gt;output_types(inputparam, [object]).&lt;&gt;image_name(inputparam, '/img/blocks/blocksheet0-_15.png').&lt;&gt;</v>
       </c>
       <c r="AI8" t="str">
         <f t="shared" si="15"/>
-        <v>[</v>
+        <v>[string</v>
       </c>
       <c r="AJ8" t="str">
         <f t="shared" si="16"/>
@@ -2398,12 +2436,18 @@
       </c>
       <c r="AP8" t="str">
         <f t="shared" si="22"/>
-        <v>[]</v>
+        <v>[string]</v>
       </c>
       <c r="AQ8" t="str">
         <f t="shared" si="23"/>
         <v>[object]</v>
       </c>
+      <c r="AS8" t="s">
+        <v>306</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>307</v>
+      </c>
       <c r="AU8">
         <v>1</v>
       </c>
@@ -2433,7 +2477,7 @@
       </c>
       <c r="BE8" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== inputparam ===========&lt;&gt;section(inputparam, 'Editor Support').&lt;&gt;subsection(inputparam, 'Editor Support').&lt;&gt;description(inputparam, 'used when defining new blocks').&lt;&gt;visual_style(inputparam,  visual_style0).&lt;&gt;inputs(inputparam, []).&lt;&gt;outputs(inputparam, ['O']).&lt;&gt;input_types(inputparam, []).&lt;&gt;output_types(inputparam, [object]).&lt;&gt;image_name(inputparam, '/img/blocks/blocksheet0-_15.png').&lt;&gt;prototype_coordinates(inputparam, 22, 4).&lt;&gt;icon_size(inputparam, 1, 1).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== inputparam ===========&lt;&gt;section(inputparam, 'Editor Support').&lt;&gt;subsection(inputparam, 'Editor Support').&lt;&gt;description(inputparam, 'used when defining new blocks').&lt;&gt;visual_style(inputparam,  visual_style0).&lt;&gt;inputs(inputparam, [required('Name')]).&lt;&gt;outputs(inputparam, ['O']).&lt;&gt;input_types(inputparam, [string]).&lt;&gt;output_types(inputparam, [object]).&lt;&gt;image_name(inputparam, '/img/blocks/blocksheet0-_15.png').&lt;&gt;prototype_coordinates(inputparam, 22, 4).&lt;&gt;icon_size(inputparam, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2451,11 +2495,16 @@
       <c r="F9" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G9" s="2" t="s">
+        <v>305</v>
+      </c>
       <c r="I9" s="3"/>
       <c r="J9" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="K9" s="10"/>
+      <c r="K9" s="10" t="s">
+        <v>162</v>
+      </c>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="4"/>
@@ -2471,7 +2520,7 @@
       </c>
       <c r="W9" s="9" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>, required('Name')</v>
       </c>
       <c r="X9" s="9" t="str">
         <f t="shared" si="5"/>
@@ -2483,7 +2532,7 @@
       </c>
       <c r="Z9" t="str">
         <f t="shared" si="7"/>
-        <v>[required('A')]</v>
+        <v>[required('A'), required('Name')]</v>
       </c>
       <c r="AA9" s="1" t="str">
         <f t="shared" si="8"/>
@@ -2515,7 +2564,7 @@
       </c>
       <c r="AH9" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== outputparam ===========&lt;&gt;section(outputparam, 'Editor Support').&lt;&gt;subsection(outputparam, 'Editor Support').&lt;&gt;description(outputparam, 'used when defining new blocks').&lt;&gt;visual_style(outputparam,  visual_style1).&lt;&gt;inputs(outputparam, [required('A')]).&lt;&gt;outputs(outputparam, []).&lt;&gt;input_types(outputparam, [object]).&lt;&gt;output_types(outputparam, []).&lt;&gt;image_name(outputparam, '/img/blocks/blocksheet0-_29.png').&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== outputparam ===========&lt;&gt;section(outputparam, 'Editor Support').&lt;&gt;subsection(outputparam, 'Editor Support').&lt;&gt;description(outputparam, 'used when defining new blocks').&lt;&gt;visual_style(outputparam,  visual_style1).&lt;&gt;inputs(outputparam, [required('A'), required('Name')]).&lt;&gt;outputs(outputparam, []).&lt;&gt;input_types(outputparam, [object, string]).&lt;&gt;output_types(outputparam, []).&lt;&gt;image_name(outputparam, '/img/blocks/blocksheet0-_29.png').&lt;&gt;</v>
       </c>
       <c r="AI9" t="str">
         <f t="shared" si="15"/>
@@ -2523,7 +2572,7 @@
       </c>
       <c r="AJ9" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>, string</v>
       </c>
       <c r="AK9" t="str">
         <f t="shared" si="17"/>
@@ -2547,12 +2596,18 @@
       </c>
       <c r="AP9" t="str">
         <f t="shared" si="22"/>
-        <v>[object]</v>
+        <v>[object, string]</v>
       </c>
       <c r="AQ9" t="str">
         <f t="shared" si="23"/>
         <v>[]</v>
       </c>
+      <c r="AS9" t="s">
+        <v>308</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>309</v>
+      </c>
       <c r="AU9">
         <v>1</v>
       </c>
@@ -2582,7 +2637,7 @@
       </c>
       <c r="BE9" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== outputparam ===========&lt;&gt;section(outputparam, 'Editor Support').&lt;&gt;subsection(outputparam, 'Editor Support').&lt;&gt;description(outputparam, 'used when defining new blocks').&lt;&gt;visual_style(outputparam,  visual_style1).&lt;&gt;inputs(outputparam, [required('A')]).&lt;&gt;outputs(outputparam, []).&lt;&gt;input_types(outputparam, [object]).&lt;&gt;output_types(outputparam, []).&lt;&gt;image_name(outputparam, '/img/blocks/blocksheet0-_29.png').&lt;&gt;prototype_coordinates(outputparam, 22, 5).&lt;&gt;icon_size(outputparam, 1, 1).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== outputparam ===========&lt;&gt;section(outputparam, 'Editor Support').&lt;&gt;subsection(outputparam, 'Editor Support').&lt;&gt;description(outputparam, 'used when defining new blocks').&lt;&gt;visual_style(outputparam,  visual_style1).&lt;&gt;inputs(outputparam, [required('A'), required('Name')]).&lt;&gt;outputs(outputparam, []).&lt;&gt;input_types(outputparam, [object, string]).&lt;&gt;output_types(outputparam, []).&lt;&gt;image_name(outputparam, '/img/blocks/blocksheet0-_29.png').&lt;&gt;prototype_coordinates(outputparam, 22, 5).&lt;&gt;icon_size(outputparam, 1, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2709,19 +2764,19 @@
         <v>27</v>
       </c>
       <c r="F11" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="J11" s="10" t="s">
-        <v>33</v>
+        <v>162</v>
       </c>
       <c r="K11" s="10" t="s">
         <v>33</v>
@@ -2743,23 +2798,23 @@
       </c>
       <c r="V11" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>[required('A')</v>
+        <v>[required('Formula')</v>
       </c>
       <c r="W11" s="9" t="str">
         <f t="shared" si="4"/>
-        <v>, required('B')</v>
+        <v>, required('A')</v>
       </c>
       <c r="X11" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>, required('C')</v>
+        <v>, required('B')</v>
       </c>
       <c r="Y11" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>, required('D')</v>
+        <v>, required('C')</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" si="7"/>
-        <v>[required('A'), required('B'), required('C')]</v>
+        <v>[required('Formula'), required('A'), required('B')]</v>
       </c>
       <c r="AA11" s="1" t="str">
         <f t="shared" si="8"/>
@@ -2791,11 +2846,11 @@
       </c>
       <c r="AH11" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;&gt;%  ===== func ===========&lt;&gt;section(func, 'Math').&lt;&gt;subsection(func, 'Math').&lt;&gt;description(func, 'This special block has a textbox for a formula. So if you type 3x+2 you see an input parameter x. Operator meaning depends on whats connected to x (scalar or vector). Understands LSL angle bracket quat syntax').&lt;&gt;visual_style(func,  normal).&lt;&gt;inputs(func, [required('A'), required('B'), required('C')]).&lt;&gt;outputs(func, ['O']).&lt;&gt;input_types(func, [scalar, scalar, scalar, scalar]).&lt;&gt;output_types(func, [object]).&lt;&gt;image_name(func, '/img/blocks/blocksheet0-_32.png').&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== func ===========&lt;&gt;section(func, 'Math').&lt;&gt;subsection(func, 'Math').&lt;&gt;description(func, 'This special block has a textbox for a formula. So if you type 3x+2 you see an input parameter x. Operator meaning depends on whats connected to x (scalar or vector). Understands LSL angle bracket quat syntax').&lt;&gt;visual_style(func,  normal).&lt;&gt;inputs(func, [required('Formula'), required('A'), required('B')]).&lt;&gt;outputs(func, ['O']).&lt;&gt;input_types(func, [string, scalar, scalar, scalar]).&lt;&gt;output_types(func, [object]).&lt;&gt;image_name(func, '/img/blocks/blocksheet0-_32.png').&lt;&gt;</v>
       </c>
       <c r="AI11" t="str">
         <f t="shared" si="15"/>
-        <v>[scalar</v>
+        <v>[string</v>
       </c>
       <c r="AJ11" t="str">
         <f t="shared" si="16"/>
@@ -2823,7 +2878,7 @@
       </c>
       <c r="AP11" t="str">
         <f t="shared" si="22"/>
-        <v>[scalar, scalar, scalar, scalar]</v>
+        <v>[string, scalar, scalar, scalar]</v>
       </c>
       <c r="AQ11" t="str">
         <f t="shared" si="23"/>
@@ -2858,7 +2913,7 @@
       </c>
       <c r="BE11" t="str">
         <f t="shared" si="24"/>
-        <v>&lt;&gt;%  ===== func ===========&lt;&gt;section(func, 'Math').&lt;&gt;subsection(func, 'Math').&lt;&gt;description(func, 'This special block has a textbox for a formula. So if you type 3x+2 you see an input parameter x. Operator meaning depends on whats connected to x (scalar or vector). Understands LSL angle bracket quat syntax').&lt;&gt;visual_style(func,  normal).&lt;&gt;inputs(func, [required('A'), required('B'), required('C')]).&lt;&gt;outputs(func, ['O']).&lt;&gt;input_types(func, [scalar, scalar, scalar, scalar]).&lt;&gt;output_types(func, [object]).&lt;&gt;image_name(func, '/img/blocks/blocksheet0-_32.png').&lt;&gt;prototype_coordinates(func, 23, 0).&lt;&gt;icon_size(func, 2, 1).&lt;&gt;</v>
+        <v>&lt;&gt;%  ===== func ===========&lt;&gt;section(func, 'Math').&lt;&gt;subsection(func, 'Math').&lt;&gt;description(func, 'This special block has a textbox for a formula. So if you type 3x+2 you see an input parameter x. Operator meaning depends on whats connected to x (scalar or vector). Understands LSL angle bracket quat syntax').&lt;&gt;visual_style(func,  normal).&lt;&gt;inputs(func, [required('Formula'), required('A'), required('B')]).&lt;&gt;outputs(func, ['O']).&lt;&gt;input_types(func, [string, scalar, scalar, scalar]).&lt;&gt;output_types(func, [object]).&lt;&gt;image_name(func, '/img/blocks/blocksheet0-_32.png').&lt;&gt;prototype_coordinates(func, 23, 0).&lt;&gt;icon_size(func, 2, 1).&lt;&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Work on blockview, working on prototype mover, added icon size to RDF
</commit_message>
<xml_diff>
--- a/doc/flo/Blocks.xlsx
+++ b/doc/flo/Blocks.xlsx
@@ -1457,12 +1457,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="11835" ySplit="495" topLeftCell="AS1" activePane="bottomLeft"/>
-      <selection activeCell="AT43" sqref="AT43"/>
+    <sheetView tabSelected="1" topLeftCell="AX1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="12120" ySplit="495" topLeftCell="BC91" activePane="bottomRight"/>
+      <selection activeCell="J11" sqref="J11"/>
       <selection pane="topRight" activeCell="BE1" sqref="BE1"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
-      <selection pane="bottomRight" activeCell="AS11" sqref="AS11"/>
+      <selection pane="bottomLeft" activeCell="AX1" sqref="AX1"/>
+      <selection pane="bottomRight" activeCell="BE100" sqref="BE100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adding CVChain support. End of day checkin, the FilterBox doesnt do anything interesting
</commit_message>
<xml_diff>
--- a/doc/flo/Blocks.xlsx
+++ b/doc/flo/Blocks.xlsx
@@ -1458,18 +1458,18 @@
   <dimension ref="A1:BE117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AX1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="12120" ySplit="495" topLeftCell="BC91" activePane="bottomRight"/>
+      <pane xSplit="12120" ySplit="495" topLeftCell="A50" activePane="bottomLeft"/>
       <selection activeCell="J11" sqref="J11"/>
       <selection pane="topRight" activeCell="BE1" sqref="BE1"/>
-      <selection pane="bottomLeft" activeCell="AX1" sqref="AX1"/>
-      <selection pane="bottomRight" activeCell="BE100" sqref="BE100"/>
+      <selection pane="bottomLeft" activeCell="BB68" sqref="BB68"/>
+      <selection pane="bottomRight" activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="17.140625" style="2"/>
     <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" style="2"/>
     <col min="6" max="9" width="8.5703125" style="2" customWidth="1"/>
     <col min="10" max="10" width="12" style="2" bestFit="1" customWidth="1"/>

</xml_diff>